<commit_message>
fixes to data git push
</commit_message>
<xml_diff>
--- a/data/First Pass Acceptance.xlsx
+++ b/data/First Pass Acceptance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\firstPassAcceptance\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,11 +23,10 @@
     <externalReference r:id="rId7"/>
     <externalReference r:id="rId8"/>
     <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Application!$A$1:$A$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FPA!$A$1:$J$177</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FPA!$A$1:$J$270</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="242">
   <si>
     <t>Project ID</t>
   </si>
@@ -462,9 +461,6 @@
     <t>Sas Micro Biasplot</t>
   </si>
   <si>
-    <t>NIck</t>
-  </si>
-  <si>
     <t>Approver List</t>
   </si>
   <si>
@@ -484,9 +480,6 @@
   </si>
   <si>
     <t>ePAS 16-38941 V3</t>
-  </si>
-  <si>
-    <t>nick</t>
   </si>
   <si>
     <t>No instruction to generate Objective Evidence</t>
@@ -1027,29 +1020,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="First Pass Acceptance"/>
-      <sheetName val="SQA"/>
-      <sheetName val="Application"/>
-      <sheetName val="Deliverable Types"/>
-      <sheetName val="Reasons for Disapproval"/>
-      <sheetName val="A or D"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="SQA"/>
       <sheetName val="Deliverable Types"/>
       <sheetName val="Application"/>
@@ -1067,7 +1037,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -1388,8 +1358,8 @@
   <dimension ref="A1:J440"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A262" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A271" sqref="A271"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3635,7 +3605,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="B79" s="21">
         <v>589.04999999999995</v>
@@ -3720,7 +3690,7 @@
         <v>28</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -3752,7 +3722,7 @@
         <v>28</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -3788,7 +3758,7 @@
         <v>39</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>135</v>
@@ -3814,7 +3784,7 @@
         <v>39</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>65</v>
@@ -3834,7 +3804,7 @@
       </c>
       <c r="I85" s="3"/>
       <c r="J85" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -3842,7 +3812,7 @@
         <v>39</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>65</v>
@@ -3862,7 +3832,7 @@
       </c>
       <c r="I86" s="3"/>
       <c r="J86" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -4008,7 +3978,7 @@
         <v>55</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
@@ -4016,7 +3986,7 @@
         <v>39</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>135</v>
@@ -4125,7 +4095,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="B96" s="3">
         <v>1075.001</v>
@@ -4556,7 +4526,7 @@
         <v>31</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
@@ -4614,7 +4584,7 @@
         <v>31</v>
       </c>
       <c r="J112" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
@@ -4674,7 +4644,7 @@
         <v>31</v>
       </c>
       <c r="J114" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
@@ -4722,7 +4692,7 @@
         <v>9</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G116" s="6" t="s">
         <v>57</v>
@@ -4732,7 +4702,7 @@
       </c>
       <c r="I116" s="3"/>
       <c r="J116" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
@@ -4762,7 +4732,7 @@
       </c>
       <c r="I117" s="3"/>
       <c r="J117" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
@@ -4792,7 +4762,7 @@
       </c>
       <c r="I118" s="3"/>
       <c r="J118" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
@@ -4812,7 +4782,7 @@
         <v>1</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G119" s="3" t="s">
         <v>58</v>
@@ -4842,7 +4812,7 @@
         <v>1</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>57</v>
@@ -4870,7 +4840,7 @@
         <v>2</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>74</v>
@@ -4898,7 +4868,7 @@
         <v>4</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G122" s="3" t="s">
         <v>58</v>
@@ -4908,7 +4878,7 @@
       </c>
       <c r="I122" s="3"/>
       <c r="J122" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
@@ -4928,7 +4898,7 @@
         <v>4</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>57</v>
@@ -4956,7 +4926,7 @@
         <v>4</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G124" s="3" t="s">
         <v>58</v>
@@ -4966,7 +4936,7 @@
       </c>
       <c r="I124" s="3"/>
       <c r="J124" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
@@ -4986,7 +4956,7 @@
         <v>4</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G125" s="3" t="s">
         <v>57</v>
@@ -5014,7 +4984,7 @@
         <v>4</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G126" s="3" t="s">
         <v>58</v>
@@ -5024,7 +4994,7 @@
       </c>
       <c r="I126" s="3"/>
       <c r="J126" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
@@ -5044,7 +5014,7 @@
         <v>4</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G127" s="3" t="s">
         <v>57</v>
@@ -5072,7 +5042,7 @@
         <v>1</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G128" s="3" t="s">
         <v>74</v>
@@ -5100,7 +5070,7 @@
         <v>1</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G129" s="3" t="s">
         <v>74</v>
@@ -5128,7 +5098,7 @@
         <v>5</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G130" s="3" t="s">
         <v>58</v>
@@ -5158,7 +5128,7 @@
         <v>5</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>57</v>
@@ -5186,7 +5156,7 @@
         <v>5</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>57</v>
@@ -5196,7 +5166,7 @@
       </c>
       <c r="I132" s="3"/>
       <c r="J132" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
@@ -5216,7 +5186,7 @@
         <v>1</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G133" s="3" t="s">
         <v>74</v>
@@ -5244,7 +5214,7 @@
         <v>1</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>57</v>
@@ -5254,7 +5224,7 @@
       </c>
       <c r="I134" s="3"/>
       <c r="J134" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
@@ -5274,7 +5244,7 @@
         <v>1</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G135" s="3" t="s">
         <v>57</v>
@@ -5284,7 +5254,7 @@
       </c>
       <c r="I135" s="3"/>
       <c r="J135" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
@@ -5304,7 +5274,7 @@
         <v>2</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G136" s="3" t="s">
         <v>74</v>
@@ -5332,7 +5302,7 @@
         <v>1</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G137" s="3" t="s">
         <v>74</v>
@@ -5348,7 +5318,7 @@
         <v>37</v>
       </c>
       <c r="B138" s="22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>51</v>
@@ -5360,7 +5330,7 @@
         <v>1</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G138" s="3" t="s">
         <v>74</v>
@@ -5388,7 +5358,7 @@
         <v>2</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G139" s="3" t="s">
         <v>74</v>
@@ -5416,7 +5386,7 @@
         <v>1</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G140" s="3" t="s">
         <v>74</v>
@@ -5444,7 +5414,7 @@
         <v>1</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G141" s="3" t="s">
         <v>58</v>
@@ -5474,7 +5444,7 @@
         <v>1</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G142" s="3" t="s">
         <v>57</v>
@@ -5502,7 +5472,7 @@
         <v>1</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G143" s="3" t="s">
         <v>58</v>
@@ -5532,7 +5502,7 @@
         <v>1</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G144" s="3" t="s">
         <v>57</v>
@@ -5560,7 +5530,7 @@
         <v>1</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G145" s="3" t="s">
         <v>58</v>
@@ -5590,7 +5560,7 @@
         <v>1</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G146" s="3" t="s">
         <v>58</v>
@@ -5620,7 +5590,7 @@
         <v>1</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G147" s="3" t="s">
         <v>58</v>
@@ -5650,7 +5620,7 @@
         <v>1</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G148" s="3" t="s">
         <v>58</v>
@@ -5680,7 +5650,7 @@
         <v>1</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G149" s="3" t="s">
         <v>58</v>
@@ -5710,7 +5680,7 @@
         <v>1</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G150" s="3" t="s">
         <v>57</v>
@@ -5738,7 +5708,7 @@
         <v>1</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G151" s="3" t="s">
         <v>58</v>
@@ -5748,7 +5718,7 @@
       </c>
       <c r="I151" s="3"/>
       <c r="J151" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
@@ -5768,7 +5738,7 @@
         <v>1</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G152" s="3" t="s">
         <v>58</v>
@@ -5798,7 +5768,7 @@
         <v>3</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G153" s="3" t="s">
         <v>74</v>
@@ -5826,7 +5796,7 @@
         <v>1</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G154" s="3" t="s">
         <v>74</v>
@@ -5854,7 +5824,7 @@
         <v>4</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G155" s="3" t="s">
         <v>74</v>
@@ -5882,7 +5852,7 @@
         <v>4</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G156" s="3" t="s">
         <v>74</v>
@@ -5910,7 +5880,7 @@
         <v>1</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G157" s="3" t="s">
         <v>74</v>
@@ -5950,7 +5920,7 @@
         <v>29</v>
       </c>
       <c r="J158" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
@@ -6026,7 +5996,7 @@
         <v>3</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G161" s="3" t="s">
         <v>58</v>
@@ -6056,7 +6026,7 @@
         <v>3</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G162" s="3" t="s">
         <v>57</v>
@@ -6066,7 +6036,7 @@
       </c>
       <c r="I162" s="3"/>
       <c r="J162" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
@@ -6086,7 +6056,7 @@
         <v>1</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G163" s="3" t="s">
         <v>74</v>
@@ -6114,7 +6084,7 @@
         <v>1</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G164" s="3" t="s">
         <v>74</v>
@@ -6142,7 +6112,7 @@
         <v>1</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G165" s="3" t="s">
         <v>58</v>
@@ -6172,7 +6142,7 @@
         <v>1</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G166" s="3" t="s">
         <v>57</v>
@@ -6200,7 +6170,7 @@
         <v>2</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G167" s="3" t="s">
         <v>57</v>
@@ -6210,7 +6180,7 @@
       </c>
       <c r="I167" s="3"/>
       <c r="J167" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
@@ -6230,7 +6200,7 @@
         <v>2</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G168" s="3" t="s">
         <v>57</v>
@@ -6240,7 +6210,7 @@
       </c>
       <c r="I168" s="3"/>
       <c r="J168" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="169" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -6260,7 +6230,7 @@
         <v>16</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G169" s="3" t="s">
         <v>58</v>
@@ -6272,7 +6242,7 @@
         <v>31</v>
       </c>
       <c r="J169" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
@@ -6292,7 +6262,7 @@
         <v>16</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G170" s="3" t="s">
         <v>57</v>
@@ -6320,7 +6290,7 @@
         <v>7</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G171" s="3" t="s">
         <v>58</v>
@@ -6350,7 +6320,7 @@
         <v>7</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G172" s="3" t="s">
         <v>57</v>
@@ -6378,7 +6348,7 @@
         <v>1</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G173" s="3" t="s">
         <v>74</v>
@@ -6406,7 +6376,7 @@
         <v>1</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G174" s="3" t="s">
         <v>74</v>
@@ -6434,7 +6404,7 @@
         <v>1</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G175" s="3" t="s">
         <v>74</v>
@@ -6462,7 +6432,7 @@
         <v>11</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G176" s="3" t="s">
         <v>74</v>
@@ -6490,7 +6460,7 @@
         <v>5</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G177" s="3" t="s">
         <v>58</v>
@@ -6508,10 +6478,10 @@
         <v>38</v>
       </c>
       <c r="B178" s="22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D178" s="3" t="s">
         <v>6</v>
@@ -6546,7 +6516,7 @@
         <v>2</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G179" s="6" t="s">
         <v>58</v>
@@ -6576,7 +6546,7 @@
         <v>3</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G180" s="6" t="s">
         <v>57</v>
@@ -6604,7 +6574,7 @@
         <v>4</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G181" s="6" t="s">
         <v>74</v>
@@ -6632,7 +6602,7 @@
         <v>4</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G182" s="6" t="s">
         <v>74</v>
@@ -6642,7 +6612,7 @@
       </c>
       <c r="I182" s="3"/>
       <c r="J182" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
@@ -6662,7 +6632,7 @@
         <v>8</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G183" s="6" t="s">
         <v>58</v>
@@ -6692,7 +6662,7 @@
         <v>8</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G184" s="6" t="s">
         <v>57</v>
@@ -6720,7 +6690,7 @@
         <v>1</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G185" s="6" t="s">
         <v>74</v>
@@ -6748,7 +6718,7 @@
         <v>5</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G186" s="6" t="s">
         <v>58</v>
@@ -6760,7 +6730,7 @@
         <v>36</v>
       </c>
       <c r="J186" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="187" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -6780,7 +6750,7 @@
         <v>5</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G187" s="6" t="s">
         <v>57</v>
@@ -6808,7 +6778,7 @@
         <v>1</v>
       </c>
       <c r="F188" s="11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G188" s="6" t="s">
         <v>57</v>
@@ -6836,7 +6806,7 @@
         <v>1</v>
       </c>
       <c r="F189" s="11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G189" s="6" t="s">
         <v>58</v>
@@ -6848,7 +6818,7 @@
         <v>36</v>
       </c>
       <c r="J189" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="190" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -6868,7 +6838,7 @@
         <v>1</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G190" s="6" t="s">
         <v>74</v>
@@ -6896,7 +6866,7 @@
         <v>1</v>
       </c>
       <c r="F191" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G191" s="6" t="s">
         <v>74</v>
@@ -6924,7 +6894,7 @@
         <v>3</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G192" s="6" t="s">
         <v>74</v>
@@ -6952,7 +6922,7 @@
         <v>1</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G193" s="6" t="s">
         <v>58</v>
@@ -6980,7 +6950,7 @@
         <v>1</v>
       </c>
       <c r="F194" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G194" s="6" t="s">
         <v>57</v>
@@ -7008,7 +6978,7 @@
         <v>1</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G195" s="6" t="s">
         <v>74</v>
@@ -7018,7 +6988,7 @@
       </c>
       <c r="I195" s="8"/>
       <c r="J195" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="196" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -7038,7 +7008,7 @@
         <v>2</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G196" s="6" t="s">
         <v>74</v>
@@ -7066,7 +7036,7 @@
         <v>1</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G197" s="6" t="s">
         <v>74</v>
@@ -7094,7 +7064,7 @@
         <v>1</v>
       </c>
       <c r="F198" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G198" s="6" t="s">
         <v>74</v>
@@ -7122,7 +7092,7 @@
         <v>1</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G199" s="6" t="s">
         <v>74</v>
@@ -7150,7 +7120,7 @@
         <v>1</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G200" s="6" t="s">
         <v>58</v>
@@ -7180,7 +7150,7 @@
         <v>1</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G201" s="6" t="s">
         <v>58</v>
@@ -7210,7 +7180,7 @@
         <v>1</v>
       </c>
       <c r="F202" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G202" s="6" t="s">
         <v>57</v>
@@ -7238,7 +7208,7 @@
         <v>1</v>
       </c>
       <c r="F203" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G203" s="6" t="s">
         <v>58</v>
@@ -7268,7 +7238,7 @@
         <v>1</v>
       </c>
       <c r="F204" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G204" s="6" t="s">
         <v>58</v>
@@ -7298,7 +7268,7 @@
         <v>1</v>
       </c>
       <c r="F205" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G205" s="6" t="s">
         <v>57</v>
@@ -7326,7 +7296,7 @@
         <v>3</v>
       </c>
       <c r="F206" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G206" s="6" t="s">
         <v>74</v>
@@ -7354,7 +7324,7 @@
         <v>1</v>
       </c>
       <c r="F207" s="25" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G207" s="6" t="s">
         <v>74</v>
@@ -7382,7 +7352,7 @@
         <v>4</v>
       </c>
       <c r="F208" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G208" s="6" t="s">
         <v>74</v>
@@ -7410,7 +7380,7 @@
         <v>2</v>
       </c>
       <c r="F209" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G209" s="6" t="s">
         <v>74</v>
@@ -7438,7 +7408,7 @@
         <v>1</v>
       </c>
       <c r="F210" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G210" s="6" t="s">
         <v>57</v>
@@ -7448,7 +7418,7 @@
       </c>
       <c r="I210" s="8"/>
       <c r="J210" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
@@ -7456,7 +7426,7 @@
         <v>37</v>
       </c>
       <c r="B211" s="24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C211" s="8" t="s">
         <v>42</v>
@@ -7468,7 +7438,7 @@
         <v>6</v>
       </c>
       <c r="F211" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G211" s="6" t="s">
         <v>74</v>
@@ -7496,7 +7466,7 @@
         <v>1</v>
       </c>
       <c r="F212" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G212" s="6" t="s">
         <v>74</v>
@@ -7524,7 +7494,7 @@
         <v>4</v>
       </c>
       <c r="F213" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G213" s="6" t="s">
         <v>74</v>
@@ -7552,7 +7522,7 @@
         <v>1</v>
       </c>
       <c r="F214" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G214" s="6" t="s">
         <v>58</v>
@@ -7582,7 +7552,7 @@
         <v>1</v>
       </c>
       <c r="F215" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G215" s="6" t="s">
         <v>57</v>
@@ -7610,7 +7580,7 @@
         <v>4</v>
       </c>
       <c r="F216" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G216" s="6" t="s">
         <v>74</v>
@@ -7638,7 +7608,7 @@
         <v>1</v>
       </c>
       <c r="F217" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G217" s="6" t="s">
         <v>57</v>
@@ -7648,7 +7618,7 @@
       </c>
       <c r="I217" s="8"/>
       <c r="J217" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="218" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -7668,7 +7638,7 @@
         <v>1</v>
       </c>
       <c r="F218" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G218" s="6" t="s">
         <v>58</v>
@@ -7698,7 +7668,7 @@
         <v>1</v>
       </c>
       <c r="F219" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G219" s="6" t="s">
         <v>58</v>
@@ -7728,7 +7698,7 @@
         <v>1</v>
       </c>
       <c r="F220" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G220" s="6" t="s">
         <v>57</v>
@@ -7756,7 +7726,7 @@
         <v>33</v>
       </c>
       <c r="F221" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G221" s="6"/>
       <c r="H221" s="10">
@@ -7782,7 +7752,7 @@
         <v>24</v>
       </c>
       <c r="F222" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G222" s="8"/>
       <c r="H222" s="10">
@@ -7818,7 +7788,7 @@
       </c>
       <c r="I223" s="8"/>
       <c r="J223" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="224" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -7838,7 +7808,7 @@
         <v>2</v>
       </c>
       <c r="F224" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G224" s="6" t="s">
         <v>74</v>
@@ -7866,7 +7836,7 @@
         <v>1</v>
       </c>
       <c r="F225" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G225" s="6" t="s">
         <v>58</v>
@@ -7878,7 +7848,7 @@
         <v>32</v>
       </c>
       <c r="J225" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="226" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -7898,7 +7868,7 @@
         <v>1</v>
       </c>
       <c r="F226" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G226" s="6" t="s">
         <v>58</v>
@@ -7928,7 +7898,7 @@
         <v>1</v>
       </c>
       <c r="F227" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G227" s="6" t="s">
         <v>57</v>
@@ -7956,7 +7926,7 @@
         <v>1</v>
       </c>
       <c r="F228" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G228" s="6" t="s">
         <v>74</v>
@@ -7984,7 +7954,7 @@
         <v>1</v>
       </c>
       <c r="F229" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G229" s="6" t="s">
         <v>74</v>
@@ -8028,7 +7998,7 @@
         <v>37</v>
       </c>
       <c r="B231" s="24" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C231" s="8" t="s">
         <v>70</v>
@@ -8048,7 +8018,7 @@
       </c>
       <c r="I231" s="8"/>
       <c r="J231" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="232" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -8068,7 +8038,7 @@
         <v>2</v>
       </c>
       <c r="F232" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G232" s="6" t="s">
         <v>74</v>
@@ -8084,7 +8054,7 @@
         <v>37</v>
       </c>
       <c r="B233" s="24" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C233" s="8" t="s">
         <v>70</v>
@@ -8122,7 +8092,7 @@
         <v>1</v>
       </c>
       <c r="F234" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G234" s="6" t="s">
         <v>74</v>
@@ -8150,7 +8120,7 @@
         <v>1</v>
       </c>
       <c r="F235" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G235" s="6" t="s">
         <v>74</v>
@@ -8188,7 +8158,7 @@
       </c>
       <c r="I236" s="3"/>
       <c r="J236" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.25">
@@ -8260,7 +8230,7 @@
         <v>64</v>
       </c>
       <c r="D239" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E239" s="3">
         <v>1</v>
@@ -8542,7 +8512,7 @@
         <v>39</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C249" s="3" t="s">
         <v>65</v>
@@ -8830,7 +8800,7 @@
         <v>39</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C259" s="3" t="s">
         <v>135</v>
@@ -8926,7 +8896,7 @@
         <v>1</v>
       </c>
       <c r="F262" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G262" s="3" t="s">
         <v>58</v>
@@ -8944,7 +8914,7 @@
         <v>39</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C263" s="3" t="s">
         <v>65</v>
@@ -8970,7 +8940,7 @@
         <v>39</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C264" s="3" t="s">
         <v>65</v>
@@ -8996,7 +8966,7 @@
         <v>39</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C265" s="3" t="s">
         <v>65</v>
@@ -9022,7 +8992,7 @@
         <v>39</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C266" s="3" t="s">
         <v>65</v>
@@ -9070,7 +9040,7 @@
       </c>
       <c r="I267" s="3"/>
       <c r="J267" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.25">
@@ -9120,7 +9090,7 @@
         <v>1</v>
       </c>
       <c r="F269" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G269" s="3" t="s">
         <v>57</v>
@@ -11243,7 +11213,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\lauernd\Desktop\[Nick First Pass Acceptance.xlsx]SQA'!#REF!</xm:f>
+            <xm:f>SQA!$A$1:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>A73:A108</xm:sqref>
         </x14:dataValidation>
@@ -11481,7 +11451,7 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -11638,7 +11608,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated data through March
</commit_message>
<xml_diff>
--- a/data/First Pass Acceptance.xlsx
+++ b/data/First Pass Acceptance.xlsx
@@ -24,7 +24,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Application!$A$1:$A$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FPA!$A$1:$J$587</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">FPA!$A$1:$J$659</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3414" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3880" uniqueCount="451">
   <si>
     <t>Project ID</t>
   </si>
@@ -1265,14 +1265,141 @@
   </si>
   <si>
     <t>ePAS 18-5711 V1</t>
+  </si>
+  <si>
+    <t>DP_Download_Protocol_v3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WWLIMS WorkStation v9.3 - LC Prod (multiple)</t>
+  </si>
+  <si>
+    <t>EDMS - Sovan Unit Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Instrument Server-v9.3 -LC PROD (multiple)</t>
+  </si>
+  <si>
+    <t>PEAR5.0.1 SAS9.4 Analysis Generation - Unit Testing</t>
+  </si>
+  <si>
+    <t>DP_Download_Protocol_v4</t>
+  </si>
+  <si>
+    <t>Fixed protocol error</t>
+  </si>
+  <si>
+    <t>Code Review - CR_Public Websites</t>
+  </si>
+  <si>
+    <t>Code Review - CR_Distributor Portal</t>
+  </si>
+  <si>
+    <t>Primary Test Protocol 1</t>
+  </si>
+  <si>
+    <t>Regression Test Protocol</t>
+  </si>
+  <si>
+    <t>Primary Test Protocol - 1l</t>
+  </si>
+  <si>
+    <t>EDMS - Sovan Unit Testing-2</t>
+  </si>
+  <si>
+    <t>EDMS-Satish Unit Testing 2</t>
+  </si>
+  <si>
+    <t>ePAS 18-6813 v1</t>
+  </si>
+  <si>
+    <t>ePAS 18-7032 v1</t>
+  </si>
+  <si>
+    <t>55.041</t>
+  </si>
+  <si>
+    <t>EDMS Unit Testing - Regression</t>
+  </si>
+  <si>
+    <t>Installation Instructions and Verification Protocol - WWLIMS WorkStation v9.3_UAT_SligoDb Migration</t>
+  </si>
+  <si>
+    <t>Installation Instructions and Verification Protocol - WWLIMS Supplemental Items v9.3 - UAT_Sligo DB Migration</t>
+  </si>
+  <si>
+    <t>User Acceptance Test Protocol - Sligo: ADDIE6D0D6303L</t>
+  </si>
+  <si>
+    <t>Installation Instructions and Verification Protocol Results: wa01924p</t>
+  </si>
+  <si>
+    <t>Primary Test Protocol - 1</t>
+  </si>
+  <si>
+    <t>Test Protocol - M1 S3 ZX and R1 Analysis Download and Output Protocol</t>
+  </si>
+  <si>
+    <t>conditional cert completed</t>
+  </si>
+  <si>
+    <t>done through email review</t>
+  </si>
+  <si>
+    <t>Installation Instructions and Verification Protocol - Instrument Manager Service(Link to v9.21)</t>
+  </si>
+  <si>
+    <t>ePAS 18-7778 V1</t>
+  </si>
+  <si>
+    <t>ePAS 16-26283 V16</t>
+  </si>
+  <si>
+    <t>ePAS 13-28491 V32</t>
+  </si>
+  <si>
+    <t>ePAS 17-4072 V15</t>
+  </si>
+  <si>
+    <t>ePAS 17-19657</t>
+  </si>
+  <si>
+    <t>ePAS 16-37034 v5</t>
+  </si>
+  <si>
+    <t>ePAS 18-9570 V1</t>
+  </si>
+  <si>
+    <t>Incomplete information</t>
+  </si>
+  <si>
+    <t>ePAS 18-7062 V1</t>
+  </si>
+  <si>
+    <t>ePAS 18-9122 v1</t>
+  </si>
+  <si>
+    <t>ePAS 18-9775 v1</t>
+  </si>
+  <si>
+    <t>Missing approvers</t>
+  </si>
+  <si>
+    <t>Missing approvers and incorrect approvers</t>
+  </si>
+  <si>
+    <t>ePAS 18-9573 V1</t>
+  </si>
+  <si>
+    <t>Power BI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1420,7 +1547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1514,6 +1641,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1841,11 +1972,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1367"/>
+  <dimension ref="A1:J1366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J587" sqref="A1:J587"/>
+      <pane ySplit="1" topLeftCell="A661" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A670" sqref="A670"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18490,998 +18621,2296 @@
       <c r="J587" s="3"/>
     </row>
     <row r="588" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A588" s="3"/>
-      <c r="B588" s="29"/>
-      <c r="C588" s="3"/>
-      <c r="D588" s="3"/>
-      <c r="E588" s="3"/>
+      <c r="A588" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B588" s="39">
+        <v>1104</v>
+      </c>
+      <c r="C588" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D588" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E588" s="3">
+        <v>1</v>
+      </c>
       <c r="F588" s="3"/>
-      <c r="G588" s="3"/>
-      <c r="H588" s="5"/>
-      <c r="I588" s="3"/>
+      <c r="G588" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H588" s="5">
+        <v>43166</v>
+      </c>
+      <c r="I588" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="J588" s="3"/>
     </row>
     <row r="589" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A589" s="3"/>
-      <c r="B589" s="29"/>
-      <c r="C589" s="3"/>
-      <c r="D589" s="3"/>
-      <c r="E589" s="3"/>
-      <c r="F589" s="3"/>
-      <c r="G589" s="3"/>
-      <c r="H589" s="5"/>
+      <c r="A589" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B589" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C589" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D589" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E589" s="3">
+        <v>3</v>
+      </c>
+      <c r="F589" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="G589" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H589" s="5">
+        <v>43161</v>
+      </c>
       <c r="I589" s="3"/>
       <c r="J589" s="3"/>
     </row>
     <row r="590" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A590" s="3"/>
-      <c r="B590" s="29"/>
-      <c r="C590" s="3"/>
-      <c r="D590" s="3"/>
-      <c r="E590" s="3"/>
-      <c r="F590" s="3"/>
-      <c r="G590" s="3"/>
-      <c r="H590" s="5"/>
+      <c r="A590" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B590" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C590" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D590" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E590" s="3">
+        <v>1</v>
+      </c>
+      <c r="F590" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="G590" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H590" s="5">
+        <v>43161</v>
+      </c>
       <c r="I590" s="3"/>
       <c r="J590" s="3"/>
     </row>
     <row r="591" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A591" s="3"/>
-      <c r="B591" s="29"/>
-      <c r="C591" s="3"/>
-      <c r="D591" s="3"/>
-      <c r="E591" s="3"/>
-      <c r="F591" s="3"/>
-      <c r="G591" s="3"/>
-      <c r="H591" s="5"/>
+      <c r="A591" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B591" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C591" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D591" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E591" s="3">
+        <v>1</v>
+      </c>
+      <c r="F591" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="G591" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H591" s="5">
+        <v>43161</v>
+      </c>
       <c r="I591" s="3"/>
       <c r="J591" s="3"/>
     </row>
     <row r="592" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A592" s="3"/>
-      <c r="B592" s="29"/>
-      <c r="C592" s="3"/>
-      <c r="D592" s="3"/>
-      <c r="E592" s="3"/>
-      <c r="F592" s="3"/>
-      <c r="G592" s="3"/>
-      <c r="H592" s="5"/>
+      <c r="A592" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B592" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C592" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D592" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E592" s="3">
+        <v>1</v>
+      </c>
+      <c r="F592" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="G592" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H592" s="5">
+        <v>43161</v>
+      </c>
       <c r="I592" s="3"/>
       <c r="J592" s="3"/>
     </row>
     <row r="593" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A593" s="3"/>
-      <c r="B593" s="29"/>
-      <c r="C593" s="3"/>
-      <c r="D593" s="3"/>
-      <c r="E593" s="3"/>
-      <c r="F593" s="3"/>
-      <c r="G593" s="3"/>
-      <c r="H593" s="5"/>
+      <c r="A593" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B593" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C593" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D593" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E593" s="3">
+        <v>3</v>
+      </c>
+      <c r="F593" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="G593" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H593" s="5">
+        <v>43161</v>
+      </c>
       <c r="I593" s="3"/>
-      <c r="J593" s="3"/>
+      <c r="J593" s="3" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="594" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A594" s="3"/>
-      <c r="B594" s="29"/>
-      <c r="C594" s="3"/>
-      <c r="D594" s="3"/>
-      <c r="E594" s="3"/>
-      <c r="F594" s="3"/>
-      <c r="G594" s="3"/>
-      <c r="H594" s="5"/>
+      <c r="A594" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B594" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C594" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D594" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E594" s="3">
+        <v>3</v>
+      </c>
+      <c r="F594" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="G594" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H594" s="5">
+        <v>43164</v>
+      </c>
       <c r="I594" s="3"/>
       <c r="J594" s="3"/>
     </row>
     <row r="595" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A595" s="3"/>
-      <c r="B595" s="29"/>
-      <c r="C595" s="3"/>
-      <c r="D595" s="3"/>
-      <c r="E595" s="3"/>
-      <c r="F595" s="3"/>
-      <c r="G595" s="3"/>
-      <c r="H595" s="5"/>
+      <c r="A595" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B595" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C595" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D595" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E595" s="3">
+        <v>3</v>
+      </c>
+      <c r="F595" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="G595" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H595" s="5">
+        <v>43164</v>
+      </c>
       <c r="I595" s="3"/>
       <c r="J595" s="3"/>
     </row>
     <row r="596" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A596" s="3"/>
-      <c r="B596" s="29"/>
-      <c r="C596" s="3"/>
-      <c r="D596" s="3"/>
-      <c r="E596" s="3"/>
-      <c r="F596" s="3"/>
-      <c r="G596" s="3"/>
-      <c r="H596" s="5"/>
+      <c r="A596" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B596" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C596" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D596" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E596" s="3">
+        <v>1</v>
+      </c>
+      <c r="F596" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="G596" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H596" s="5">
+        <v>43164</v>
+      </c>
       <c r="I596" s="3"/>
       <c r="J596" s="3"/>
     </row>
     <row r="597" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A597" s="3"/>
-      <c r="B597" s="29"/>
-      <c r="C597" s="3"/>
-      <c r="D597" s="3"/>
-      <c r="E597" s="3"/>
-      <c r="F597" s="3"/>
-      <c r="G597" s="3"/>
-      <c r="H597" s="5"/>
+      <c r="A597" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B597" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C597" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D597" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E597" s="3">
+        <v>1</v>
+      </c>
+      <c r="F597" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="G597" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H597" s="5">
+        <v>43164</v>
+      </c>
       <c r="I597" s="3"/>
       <c r="J597" s="3"/>
     </row>
     <row r="598" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A598" s="3"/>
-      <c r="B598" s="29"/>
-      <c r="C598" s="3"/>
-      <c r="D598" s="3"/>
-      <c r="E598" s="3"/>
-      <c r="F598" s="3"/>
-      <c r="G598" s="3"/>
-      <c r="H598" s="5"/>
+      <c r="A598" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B598" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C598" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D598" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E598" s="3">
+        <v>1</v>
+      </c>
+      <c r="F598" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="G598" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H598" s="5">
+        <v>43164</v>
+      </c>
       <c r="I598" s="3"/>
       <c r="J598" s="3"/>
     </row>
     <row r="599" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A599" s="3"/>
-      <c r="B599" s="29"/>
-      <c r="C599" s="3"/>
-      <c r="D599" s="3"/>
-      <c r="E599" s="3"/>
-      <c r="F599" s="3"/>
-      <c r="G599" s="3"/>
-      <c r="H599" s="5"/>
+      <c r="A599" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B599" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C599" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D599" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E599" s="3">
+        <v>1</v>
+      </c>
+      <c r="F599" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="G599" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H599" s="5">
+        <v>43164</v>
+      </c>
       <c r="I599" s="3"/>
       <c r="J599" s="3"/>
     </row>
     <row r="600" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A600" s="3"/>
-      <c r="B600" s="29"/>
-      <c r="C600" s="3"/>
-      <c r="D600" s="3"/>
-      <c r="E600" s="3"/>
-      <c r="F600" s="3"/>
-      <c r="G600" s="3"/>
-      <c r="H600" s="5"/>
+      <c r="A600" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B600" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C600" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D600" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E600" s="3">
+        <v>4</v>
+      </c>
+      <c r="F600" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="G600" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H600" s="5">
+        <v>43164</v>
+      </c>
       <c r="I600" s="3"/>
-      <c r="J600" s="3"/>
+      <c r="J600" s="3" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="601" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A601" s="3"/>
-      <c r="B601" s="29"/>
-      <c r="C601" s="3"/>
-      <c r="D601" s="3"/>
-      <c r="E601" s="3"/>
-      <c r="F601" s="3"/>
-      <c r="G601" s="3"/>
-      <c r="H601" s="5"/>
+      <c r="A601" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B601" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C601" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D601" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E601" s="3">
+        <v>3</v>
+      </c>
+      <c r="F601" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G601" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H601" s="5">
+        <v>43164</v>
+      </c>
       <c r="I601" s="3"/>
       <c r="J601" s="3"/>
     </row>
     <row r="602" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A602" s="3"/>
-      <c r="B602" s="29"/>
-      <c r="C602" s="3"/>
-      <c r="D602" s="3"/>
-      <c r="E602" s="3"/>
-      <c r="F602" s="3"/>
-      <c r="G602" s="3"/>
-      <c r="H602" s="5"/>
+      <c r="A602" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B602" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C602" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D602" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E602" s="3">
+        <v>4</v>
+      </c>
+      <c r="F602" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G602" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H602" s="5">
+        <v>43165</v>
+      </c>
       <c r="I602" s="3"/>
       <c r="J602" s="3"/>
     </row>
     <row r="603" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A603" s="3"/>
-      <c r="B603" s="29"/>
-      <c r="C603" s="3"/>
-      <c r="D603" s="3"/>
-      <c r="E603" s="3"/>
-      <c r="F603" s="3"/>
-      <c r="G603" s="3"/>
-      <c r="H603" s="5"/>
+      <c r="A603" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B603" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C603" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D603" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E603" s="3">
+        <v>2</v>
+      </c>
+      <c r="F603" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="G603" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H603" s="5">
+        <v>43165</v>
+      </c>
       <c r="I603" s="3"/>
       <c r="J603" s="3"/>
     </row>
     <row r="604" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A604" s="3"/>
-      <c r="B604" s="29"/>
-      <c r="C604" s="3"/>
-      <c r="D604" s="3"/>
-      <c r="E604" s="3"/>
-      <c r="F604" s="3"/>
-      <c r="G604" s="3"/>
-      <c r="H604" s="5"/>
+      <c r="A604" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B604" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C604" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D604" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E604" s="3">
+        <v>1</v>
+      </c>
+      <c r="F604" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="G604" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H604" s="5">
+        <v>43166</v>
+      </c>
       <c r="I604" s="3"/>
       <c r="J604" s="3"/>
     </row>
     <row r="605" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A605" s="3"/>
-      <c r="B605" s="29"/>
-      <c r="C605" s="3"/>
-      <c r="D605" s="3"/>
-      <c r="E605" s="3"/>
-      <c r="F605" s="3"/>
-      <c r="G605" s="3"/>
-      <c r="H605" s="5"/>
+      <c r="A605" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B605" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C605" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D605" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E605" s="3">
+        <v>1</v>
+      </c>
+      <c r="F605" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="G605" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H605" s="5">
+        <v>43166</v>
+      </c>
       <c r="I605" s="3"/>
       <c r="J605" s="3"/>
     </row>
     <row r="606" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A606" s="3"/>
-      <c r="B606" s="29"/>
-      <c r="C606" s="3"/>
-      <c r="D606" s="3"/>
-      <c r="E606" s="3"/>
+      <c r="A606" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B606" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C606" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D606" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E606" s="3">
+        <v>1</v>
+      </c>
       <c r="F606" s="3"/>
-      <c r="G606" s="3"/>
-      <c r="H606" s="5"/>
-      <c r="I606" s="3"/>
+      <c r="G606" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H606" s="5">
+        <v>43166</v>
+      </c>
+      <c r="I606" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="J606" s="3"/>
     </row>
     <row r="607" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A607" s="3"/>
-      <c r="B607" s="29"/>
-      <c r="C607" s="3"/>
-      <c r="D607" s="3"/>
-      <c r="E607" s="3"/>
+      <c r="A607" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B607" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C607" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D607" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E607" s="3">
+        <v>1</v>
+      </c>
       <c r="F607" s="3"/>
-      <c r="G607" s="3"/>
-      <c r="H607" s="5"/>
+      <c r="G607" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H607" s="5">
+        <v>43166</v>
+      </c>
       <c r="I607" s="3"/>
       <c r="J607" s="3"/>
     </row>
     <row r="608" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A608" s="3"/>
-      <c r="B608" s="29"/>
-      <c r="C608" s="3"/>
-      <c r="D608" s="3"/>
-      <c r="E608" s="3"/>
+      <c r="A608" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B608" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C608" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D608" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E608" s="3">
+        <v>1</v>
+      </c>
       <c r="F608" s="3"/>
-      <c r="G608" s="3"/>
-      <c r="H608" s="5"/>
+      <c r="G608" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H608" s="5">
+        <v>43167</v>
+      </c>
       <c r="I608" s="3"/>
       <c r="J608" s="3"/>
     </row>
     <row r="609" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A609" s="3"/>
-      <c r="B609" s="29"/>
-      <c r="C609" s="3"/>
-      <c r="D609" s="3"/>
-      <c r="E609" s="3"/>
-      <c r="F609" s="3"/>
-      <c r="G609" s="3"/>
-      <c r="H609" s="5"/>
+      <c r="A609" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B609" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C609" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D609" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E609" s="3">
+        <v>1</v>
+      </c>
+      <c r="F609" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="G609" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H609" s="5">
+        <v>43167</v>
+      </c>
       <c r="I609" s="3"/>
       <c r="J609" s="3"/>
     </row>
     <row r="610" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A610" s="3"/>
-      <c r="B610" s="29"/>
-      <c r="C610" s="3"/>
-      <c r="D610" s="3"/>
-      <c r="E610" s="3"/>
-      <c r="F610" s="3"/>
-      <c r="G610" s="3"/>
-      <c r="H610" s="5"/>
+      <c r="A610" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B610" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C610" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D610" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E610" s="3">
+        <v>1</v>
+      </c>
+      <c r="F610" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="G610" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H610" s="5">
+        <v>43167</v>
+      </c>
       <c r="I610" s="3"/>
-      <c r="J610" s="3"/>
+      <c r="J610" s="3" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="611" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A611" s="3"/>
-      <c r="B611" s="29"/>
-      <c r="C611" s="3"/>
-      <c r="D611" s="3"/>
-      <c r="E611" s="3"/>
+      <c r="A611" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B611" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C611" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D611" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E611" s="3">
+        <v>1</v>
+      </c>
       <c r="F611" s="3"/>
-      <c r="G611" s="3"/>
-      <c r="H611" s="5"/>
+      <c r="G611" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H611" s="5">
+        <v>43167</v>
+      </c>
       <c r="I611" s="3"/>
       <c r="J611" s="3"/>
     </row>
     <row r="612" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A612" s="3"/>
-      <c r="B612" s="29"/>
-      <c r="C612" s="3"/>
-      <c r="D612" s="3"/>
-      <c r="E612" s="3"/>
-      <c r="F612" s="3"/>
-      <c r="G612" s="3"/>
-      <c r="H612" s="5"/>
+      <c r="A612" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B612" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C612" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D612" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E612" s="3">
+        <v>1</v>
+      </c>
+      <c r="F612" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="G612" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H612" s="5">
+        <v>43167</v>
+      </c>
       <c r="I612" s="3"/>
       <c r="J612" s="3"/>
     </row>
     <row r="613" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A613" s="3"/>
-      <c r="B613" s="29"/>
-      <c r="C613" s="3"/>
-      <c r="D613" s="3"/>
-      <c r="E613" s="3"/>
-      <c r="F613" s="3"/>
-      <c r="G613" s="3"/>
-      <c r="H613" s="5"/>
+      <c r="A613" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B613" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C613" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D613" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E613" s="3">
+        <v>1</v>
+      </c>
+      <c r="F613" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="G613" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H613" s="5">
+        <v>43167</v>
+      </c>
       <c r="I613" s="3"/>
       <c r="J613" s="3"/>
     </row>
     <row r="614" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A614" s="3"/>
-      <c r="B614" s="29"/>
-      <c r="C614" s="3"/>
-      <c r="D614" s="3"/>
-      <c r="E614" s="3"/>
-      <c r="F614" s="3"/>
-      <c r="G614" s="3"/>
-      <c r="H614" s="5"/>
+      <c r="A614" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B614" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C614" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D614" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E614" s="3">
+        <v>1</v>
+      </c>
+      <c r="F614" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="G614" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H614" s="5">
+        <v>43167</v>
+      </c>
       <c r="I614" s="3"/>
       <c r="J614" s="3"/>
     </row>
     <row r="615" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A615" s="3"/>
-      <c r="B615" s="29"/>
-      <c r="C615" s="3"/>
-      <c r="D615" s="3"/>
-      <c r="E615" s="3"/>
-      <c r="F615" s="3"/>
-      <c r="G615" s="3"/>
-      <c r="H615" s="5"/>
+      <c r="A615" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B615" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C615" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D615" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E615" s="3">
+        <v>1</v>
+      </c>
+      <c r="F615" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="G615" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H615" s="5">
+        <v>43167</v>
+      </c>
       <c r="I615" s="3"/>
       <c r="J615" s="3"/>
     </row>
     <row r="616" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A616" s="3"/>
-      <c r="B616" s="29"/>
-      <c r="C616" s="3"/>
-      <c r="D616" s="3"/>
-      <c r="E616" s="3"/>
-      <c r="F616" s="3"/>
-      <c r="G616" s="3"/>
-      <c r="H616" s="5"/>
-      <c r="I616" s="3"/>
+      <c r="A616" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B616" s="29">
+        <v>500.06</v>
+      </c>
+      <c r="C616" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D616" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E616" s="3">
+        <v>1</v>
+      </c>
+      <c r="F616" s="3">
+        <v>1</v>
+      </c>
+      <c r="G616" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H616" s="5">
+        <v>43164</v>
+      </c>
+      <c r="I616" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="J616" s="3"/>
     </row>
     <row r="617" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A617" s="3"/>
-      <c r="B617" s="29"/>
-      <c r="C617" s="3"/>
-      <c r="D617" s="3"/>
-      <c r="E617" s="3"/>
+      <c r="A617" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B617" s="29" t="s">
+        <v>423</v>
+      </c>
+      <c r="C617" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D617" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E617" s="3">
+        <v>4.2</v>
+      </c>
       <c r="F617" s="3"/>
-      <c r="G617" s="3"/>
-      <c r="H617" s="5"/>
+      <c r="G617" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H617" s="5">
+        <v>43166</v>
+      </c>
       <c r="I617" s="3"/>
       <c r="J617" s="3"/>
     </row>
     <row r="618" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A618" s="3"/>
-      <c r="B618" s="29"/>
-      <c r="C618" s="3"/>
-      <c r="D618" s="3"/>
-      <c r="E618" s="3"/>
-      <c r="F618" s="3"/>
-      <c r="G618" s="3"/>
-      <c r="H618" s="5"/>
-      <c r="I618" s="3"/>
+      <c r="A618" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B618" s="29">
+        <v>500.06</v>
+      </c>
+      <c r="C618" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D618" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E618" s="3">
+        <v>1</v>
+      </c>
+      <c r="F618" s="3">
+        <v>1</v>
+      </c>
+      <c r="G618" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H618" s="5">
+        <v>43166</v>
+      </c>
+      <c r="I618" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="J618" s="3"/>
     </row>
     <row r="619" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A619" s="3"/>
-      <c r="B619" s="29"/>
-      <c r="C619" s="3"/>
-      <c r="D619" s="3"/>
-      <c r="E619" s="3"/>
-      <c r="F619" s="3"/>
-      <c r="G619" s="3"/>
-      <c r="H619" s="5"/>
+      <c r="A619" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B619" s="29">
+        <v>500.06</v>
+      </c>
+      <c r="C619" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D619" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E619" s="3">
+        <v>1</v>
+      </c>
+      <c r="F619" s="3">
+        <v>1</v>
+      </c>
+      <c r="G619" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H619" s="5">
+        <v>43166</v>
+      </c>
       <c r="I619" s="3"/>
       <c r="J619" s="3"/>
     </row>
     <row r="620" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A620" s="3"/>
-      <c r="B620" s="29"/>
-      <c r="C620" s="3"/>
-      <c r="D620" s="3"/>
-      <c r="E620" s="3"/>
+      <c r="A620" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B620" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="C620" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D620" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E620" s="3">
+        <v>1</v>
+      </c>
       <c r="F620" s="3"/>
-      <c r="G620" s="3"/>
-      <c r="H620" s="5"/>
+      <c r="G620" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H620" s="5">
+        <v>43167</v>
+      </c>
       <c r="I620" s="3"/>
       <c r="J620" s="3"/>
     </row>
     <row r="621" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A621" s="3"/>
-      <c r="B621" s="29"/>
-      <c r="C621" s="3"/>
-      <c r="D621" s="3"/>
-      <c r="E621" s="3"/>
-      <c r="F621" s="3"/>
-      <c r="G621" s="3"/>
-      <c r="H621" s="5"/>
+      <c r="A621" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B621" s="29">
+        <v>500.03800000000001</v>
+      </c>
+      <c r="C621" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D621" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E621" s="3">
+        <v>1</v>
+      </c>
+      <c r="F621" s="3">
+        <v>1</v>
+      </c>
+      <c r="G621" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H621" s="5">
+        <v>43168</v>
+      </c>
       <c r="I621" s="3"/>
       <c r="J621" s="3"/>
     </row>
     <row r="622" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A622" s="3"/>
-      <c r="B622" s="29"/>
-      <c r="C622" s="3"/>
-      <c r="D622" s="3"/>
-      <c r="E622" s="3"/>
+      <c r="A622" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B622" s="29">
+        <v>55.040999999999997</v>
+      </c>
+      <c r="C622" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D622" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E622" s="3">
+        <v>1</v>
+      </c>
       <c r="F622" s="3"/>
-      <c r="G622" s="3"/>
-      <c r="H622" s="5"/>
-      <c r="I622" s="3"/>
+      <c r="G622" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H622" s="5">
+        <v>43172</v>
+      </c>
+      <c r="I622" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="J622" s="3"/>
     </row>
     <row r="623" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A623" s="3"/>
-      <c r="B623" s="29"/>
-      <c r="C623" s="3"/>
-      <c r="D623" s="3"/>
-      <c r="E623" s="3"/>
+      <c r="A623" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B623" s="40" t="s">
+        <v>425</v>
+      </c>
+      <c r="C623" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D623" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E623" s="3">
+        <v>1</v>
+      </c>
       <c r="F623" s="3"/>
-      <c r="G623" s="3"/>
-      <c r="H623" s="5"/>
+      <c r="G623" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H623" s="5">
+        <v>43173</v>
+      </c>
       <c r="I623" s="3"/>
       <c r="J623" s="3"/>
     </row>
     <row r="624" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A624" s="3"/>
-      <c r="B624" s="29"/>
-      <c r="C624" s="3"/>
-      <c r="D624" s="3"/>
-      <c r="E624" s="3"/>
+      <c r="A624" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B624" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C624" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D624" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E624" s="3">
+        <v>1</v>
+      </c>
       <c r="F624" s="3"/>
-      <c r="G624" s="3"/>
-      <c r="H624" s="5"/>
+      <c r="G624" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H624" s="5">
+        <v>43174</v>
+      </c>
       <c r="I624" s="3"/>
       <c r="J624" s="3"/>
     </row>
     <row r="625" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A625" s="3"/>
-      <c r="B625" s="29"/>
-      <c r="C625" s="3"/>
-      <c r="D625" s="3"/>
-      <c r="E625" s="3"/>
-      <c r="F625" s="3"/>
-      <c r="G625" s="3"/>
-      <c r="H625" s="5"/>
+      <c r="A625" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B625" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C625" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D625" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E625" s="3">
+        <v>1</v>
+      </c>
+      <c r="F625" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="G625" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H625" s="5">
+        <v>43171</v>
+      </c>
       <c r="I625" s="3"/>
       <c r="J625" s="3"/>
     </row>
     <row r="626" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A626" s="3"/>
-      <c r="B626" s="29"/>
-      <c r="C626" s="3"/>
-      <c r="D626" s="3"/>
-      <c r="E626" s="3"/>
-      <c r="F626" s="3"/>
-      <c r="G626" s="3"/>
-      <c r="H626" s="5"/>
+      <c r="A626" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B626" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C626" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D626" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E626" s="3">
+        <v>1</v>
+      </c>
+      <c r="F626" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="G626" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H626" s="5">
+        <v>43171</v>
+      </c>
       <c r="I626" s="3"/>
-      <c r="J626" s="3"/>
+      <c r="J626" s="3" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="627" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A627" s="3"/>
-      <c r="B627" s="29"/>
-      <c r="C627" s="3"/>
-      <c r="D627" s="3"/>
-      <c r="E627" s="3"/>
-      <c r="F627" s="3"/>
-      <c r="G627" s="3"/>
-      <c r="H627" s="5"/>
+      <c r="A627" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B627" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C627" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D627" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E627" s="3">
+        <v>1</v>
+      </c>
+      <c r="F627" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G627" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H627" s="5">
+        <v>43171</v>
+      </c>
       <c r="I627" s="3"/>
       <c r="J627" s="3"/>
     </row>
     <row r="628" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A628" s="3"/>
-      <c r="B628" s="29"/>
-      <c r="C628" s="3"/>
-      <c r="D628" s="3"/>
-      <c r="E628" s="3"/>
-      <c r="F628" s="3"/>
-      <c r="G628" s="3"/>
-      <c r="H628" s="5"/>
-      <c r="I628" s="3"/>
+      <c r="A628" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B628" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C628" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D628" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E628" s="3">
+        <v>1</v>
+      </c>
+      <c r="F628" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="G628" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H628" s="5">
+        <v>43172</v>
+      </c>
+      <c r="I628" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="J628" s="3"/>
     </row>
     <row r="629" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A629" s="3"/>
-      <c r="B629" s="29"/>
-      <c r="C629" s="3"/>
-      <c r="D629" s="3"/>
-      <c r="E629" s="3"/>
-      <c r="F629" s="3"/>
-      <c r="G629" s="3"/>
-      <c r="H629" s="5"/>
+      <c r="A629" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B629" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C629" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D629" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E629" s="3">
+        <v>1</v>
+      </c>
+      <c r="F629" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="G629" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H629" s="5">
+        <v>43173</v>
+      </c>
       <c r="I629" s="3"/>
       <c r="J629" s="3"/>
     </row>
     <row r="630" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A630" s="3"/>
-      <c r="B630" s="29"/>
-      <c r="C630" s="3"/>
-      <c r="D630" s="3"/>
-      <c r="E630" s="3"/>
-      <c r="F630" s="3"/>
-      <c r="G630" s="3"/>
-      <c r="H630" s="5"/>
+      <c r="A630" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B630" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C630" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D630" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E630" s="3">
+        <v>1</v>
+      </c>
+      <c r="F630" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="G630" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H630" s="5">
+        <v>43173</v>
+      </c>
       <c r="I630" s="3"/>
       <c r="J630" s="3"/>
     </row>
     <row r="631" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A631" s="3"/>
-      <c r="B631" s="29"/>
-      <c r="C631" s="3"/>
-      <c r="D631" s="3"/>
-      <c r="E631" s="3"/>
-      <c r="F631" s="3"/>
-      <c r="G631" s="3"/>
-      <c r="H631" s="5"/>
+      <c r="A631" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B631" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="C631" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D631" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E631" s="3">
+        <v>1</v>
+      </c>
+      <c r="F631" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="G631" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H631" s="5">
+        <v>43174</v>
+      </c>
       <c r="I631" s="3"/>
       <c r="J631" s="3"/>
     </row>
     <row r="632" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A632" s="3"/>
-      <c r="B632" s="29"/>
-      <c r="C632" s="3"/>
-      <c r="D632" s="3"/>
-      <c r="E632" s="3"/>
-      <c r="F632" s="3"/>
-      <c r="G632" s="3"/>
-      <c r="H632" s="5"/>
+      <c r="A632" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B632" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C632" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D632" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E632" s="3">
+        <v>1</v>
+      </c>
+      <c r="F632" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="G632" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H632" s="5">
+        <v>43178</v>
+      </c>
       <c r="I632" s="3"/>
       <c r="J632" s="3"/>
     </row>
     <row r="633" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A633" s="3"/>
-      <c r="B633" s="29"/>
-      <c r="C633" s="3"/>
-      <c r="D633" s="3"/>
-      <c r="E633" s="3"/>
-      <c r="F633" s="3"/>
-      <c r="G633" s="3"/>
-      <c r="H633" s="5"/>
+      <c r="A633" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B633" s="29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C633" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D633" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E633" s="3">
+        <v>1</v>
+      </c>
+      <c r="F633" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="G633" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H633" s="5">
+        <v>43178</v>
+      </c>
       <c r="I633" s="3"/>
-      <c r="J633" s="3"/>
+      <c r="J633" s="3" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="634" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A634" s="3"/>
-      <c r="B634" s="29"/>
-      <c r="C634" s="3"/>
-      <c r="D634" s="3"/>
-      <c r="E634" s="3"/>
+      <c r="A634" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B634" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="C634" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D634" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E634" s="3">
+        <v>3</v>
+      </c>
       <c r="F634" s="3"/>
-      <c r="G634" s="3"/>
-      <c r="H634" s="5"/>
+      <c r="G634" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H634" s="5">
+        <v>43178</v>
+      </c>
       <c r="I634" s="3"/>
-      <c r="J634" s="3"/>
+      <c r="J634" s="3" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="635" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A635" s="3"/>
-      <c r="B635" s="29"/>
-      <c r="C635" s="3"/>
-      <c r="D635" s="3"/>
-      <c r="E635" s="3"/>
-      <c r="F635" s="3"/>
-      <c r="G635" s="3"/>
-      <c r="H635" s="5"/>
+      <c r="A635" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B635" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="C635" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D635" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E635" s="3">
+        <v>1</v>
+      </c>
+      <c r="F635" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="G635" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H635" s="5">
+        <v>43180</v>
+      </c>
       <c r="I635" s="3"/>
       <c r="J635" s="3"/>
     </row>
     <row r="636" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A636" s="3"/>
-      <c r="B636" s="29"/>
-      <c r="C636" s="3"/>
-      <c r="D636" s="3"/>
-      <c r="E636" s="3"/>
+      <c r="A636" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B636" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="C636" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D636" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E636" s="3">
+        <v>1</v>
+      </c>
       <c r="F636" s="3"/>
-      <c r="G636" s="3"/>
-      <c r="H636" s="5"/>
+      <c r="G636" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H636" s="5">
+        <v>43180</v>
+      </c>
       <c r="I636" s="3"/>
       <c r="J636" s="3"/>
     </row>
     <row r="637" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A637" s="3"/>
-      <c r="B637" s="29"/>
-      <c r="C637" s="3"/>
-      <c r="D637" s="3"/>
-      <c r="E637" s="3"/>
+      <c r="A637" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B637" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="C637" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D637" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E637" s="3">
+        <v>2</v>
+      </c>
       <c r="F637" s="3"/>
-      <c r="G637" s="3"/>
-      <c r="H637" s="5"/>
-      <c r="I637" s="3"/>
-      <c r="J637" s="3"/>
+      <c r="G637" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H637" s="5">
+        <v>43180</v>
+      </c>
+      <c r="I637" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J637" s="3" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="638" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A638" s="3"/>
-      <c r="B638" s="29"/>
-      <c r="C638" s="3"/>
-      <c r="D638" s="3"/>
-      <c r="E638" s="3"/>
+      <c r="A638" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B638" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="C638" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D638" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E638" s="3">
+        <v>2</v>
+      </c>
       <c r="F638" s="3"/>
-      <c r="G638" s="3"/>
-      <c r="H638" s="5"/>
+      <c r="G638" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H638" s="5">
+        <v>43180</v>
+      </c>
       <c r="I638" s="3"/>
       <c r="J638" s="3"/>
     </row>
     <row r="639" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A639" s="3"/>
-      <c r="B639" s="29"/>
-      <c r="C639" s="3"/>
-      <c r="D639" s="3"/>
-      <c r="E639" s="3"/>
+      <c r="A639" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B639" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C639" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D639" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E639" s="3">
+        <v>2</v>
+      </c>
       <c r="F639" s="3"/>
-      <c r="G639" s="3"/>
-      <c r="H639" s="5"/>
-      <c r="I639" s="3"/>
-      <c r="J639" s="3"/>
+      <c r="G639" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H639" s="5">
+        <v>43180</v>
+      </c>
+      <c r="I639" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J639" s="3" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="640" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A640" s="3"/>
-      <c r="B640" s="29"/>
-      <c r="C640" s="3"/>
-      <c r="D640" s="3"/>
-      <c r="E640" s="3"/>
+      <c r="A640" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B640" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C640" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D640" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E640" s="3">
+        <v>2</v>
+      </c>
       <c r="F640" s="3"/>
-      <c r="G640" s="3"/>
-      <c r="H640" s="5"/>
+      <c r="G640" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H640" s="5">
+        <v>43181</v>
+      </c>
       <c r="I640" s="3"/>
       <c r="J640" s="3"/>
     </row>
     <row r="641" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A641" s="3"/>
-      <c r="B641" s="29"/>
-      <c r="C641" s="3"/>
-      <c r="D641" s="3"/>
-      <c r="E641" s="3"/>
-      <c r="F641" s="3"/>
-      <c r="G641" s="3"/>
-      <c r="H641" s="5"/>
+      <c r="A641" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B641" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C641" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D641" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E641" s="3">
+        <v>2</v>
+      </c>
+      <c r="F641" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="G641" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H641" s="5">
+        <v>43180</v>
+      </c>
       <c r="I641" s="3"/>
-      <c r="J641" s="3"/>
+      <c r="J641" s="3" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="642" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A642" s="3"/>
-      <c r="B642" s="29"/>
-      <c r="C642" s="3"/>
-      <c r="D642" s="3"/>
-      <c r="E642" s="3"/>
+      <c r="A642" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B642" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="C642" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D642" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E642" s="3">
+        <v>1</v>
+      </c>
       <c r="F642" s="3"/>
-      <c r="G642" s="3"/>
-      <c r="H642" s="5"/>
+      <c r="G642" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H642" s="5">
+        <v>43171</v>
+      </c>
       <c r="I642" s="3"/>
       <c r="J642" s="3"/>
     </row>
     <row r="643" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A643" s="3"/>
-      <c r="B643" s="29"/>
-      <c r="C643" s="3"/>
-      <c r="D643" s="3"/>
-      <c r="E643" s="3"/>
+      <c r="A643" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B643" s="29" t="s">
+        <v>437</v>
+      </c>
+      <c r="C643" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D643" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E643" s="3">
+        <v>1</v>
+      </c>
       <c r="F643" s="3"/>
-      <c r="G643" s="3"/>
-      <c r="H643" s="5"/>
+      <c r="G643" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H643" s="5">
+        <v>43171</v>
+      </c>
       <c r="I643" s="3"/>
       <c r="J643" s="3"/>
     </row>
     <row r="644" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A644" s="3"/>
-      <c r="B644" s="29"/>
-      <c r="C644" s="3"/>
-      <c r="D644" s="3"/>
-      <c r="E644" s="3"/>
+      <c r="A644" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B644" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="C644" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D644" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E644" s="3">
+        <v>1</v>
+      </c>
       <c r="F644" s="3"/>
-      <c r="G644" s="3"/>
-      <c r="H644" s="5"/>
+      <c r="G644" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H644" s="5">
+        <v>43173</v>
+      </c>
       <c r="I644" s="3"/>
       <c r="J644" s="3"/>
     </row>
     <row r="645" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A645" s="3"/>
-      <c r="B645" s="29"/>
-      <c r="C645" s="3"/>
-      <c r="D645" s="3"/>
-      <c r="E645" s="3"/>
+      <c r="A645" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B645" s="29" t="s">
+        <v>438</v>
+      </c>
+      <c r="C645" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D645" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E645" s="3">
+        <v>1</v>
+      </c>
       <c r="F645" s="3"/>
-      <c r="G645" s="3"/>
-      <c r="H645" s="5"/>
+      <c r="G645" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H645" s="5">
+        <v>43173</v>
+      </c>
       <c r="I645" s="3"/>
       <c r="J645" s="3"/>
     </row>
     <row r="646" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A646" s="3"/>
-      <c r="B646" s="29"/>
-      <c r="C646" s="3"/>
-      <c r="D646" s="3"/>
-      <c r="E646" s="3"/>
+      <c r="A646" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B646" s="29" t="s">
+        <v>439</v>
+      </c>
+      <c r="C646" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D646" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E646" s="3">
+        <v>1</v>
+      </c>
       <c r="F646" s="3"/>
-      <c r="G646" s="3"/>
-      <c r="H646" s="5"/>
+      <c r="G646" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H646" s="5">
+        <v>43174</v>
+      </c>
       <c r="I646" s="3"/>
       <c r="J646" s="3"/>
     </row>
     <row r="647" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A647" s="3"/>
-      <c r="B647" s="29"/>
-      <c r="C647" s="3"/>
-      <c r="D647" s="3"/>
-      <c r="E647" s="3"/>
-      <c r="F647" s="3"/>
-      <c r="G647" s="3"/>
-      <c r="H647" s="5"/>
-      <c r="I647" s="3"/>
+      <c r="A647" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B647" s="29">
+        <v>771.00900000000001</v>
+      </c>
+      <c r="C647" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D647" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E647" s="3">
+        <v>1</v>
+      </c>
+      <c r="F647" s="3">
+        <v>1</v>
+      </c>
+      <c r="G647" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H647" s="5">
+        <v>43175</v>
+      </c>
+      <c r="I647" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="J647" s="3"/>
     </row>
     <row r="648" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A648" s="3"/>
-      <c r="B648" s="29"/>
-      <c r="C648" s="3"/>
-      <c r="D648" s="3"/>
-      <c r="E648" s="3"/>
-      <c r="F648" s="3"/>
-      <c r="G648" s="3"/>
-      <c r="H648" s="5"/>
-      <c r="I648" s="3"/>
+      <c r="A648" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B648" s="29">
+        <v>771.00900000000001</v>
+      </c>
+      <c r="C648" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D648" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E648" s="3">
+        <v>1</v>
+      </c>
+      <c r="F648" s="3">
+        <v>1</v>
+      </c>
+      <c r="G648" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H648" s="5">
+        <v>43178</v>
+      </c>
+      <c r="I648" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="J648" s="3"/>
     </row>
     <row r="649" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A649" s="3"/>
-      <c r="B649" s="29"/>
-      <c r="C649" s="3"/>
-      <c r="D649" s="3"/>
-      <c r="E649" s="3"/>
-      <c r="F649" s="3"/>
-      <c r="G649" s="3"/>
-      <c r="H649" s="5"/>
+      <c r="A649" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B649" s="29">
+        <v>771.00900000000001</v>
+      </c>
+      <c r="C649" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D649" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E649" s="3">
+        <v>1</v>
+      </c>
+      <c r="F649" s="3">
+        <v>1</v>
+      </c>
+      <c r="G649" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H649" s="5">
+        <v>43180</v>
+      </c>
       <c r="I649" s="3"/>
       <c r="J649" s="3"/>
     </row>
     <row r="650" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A650" s="3"/>
-      <c r="B650" s="29"/>
-      <c r="C650" s="3"/>
-      <c r="D650" s="3"/>
-      <c r="E650" s="3"/>
+      <c r="A650" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B650" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C650" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D650" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E650" s="3">
+        <v>1</v>
+      </c>
       <c r="F650" s="3"/>
-      <c r="G650" s="3"/>
-      <c r="H650" s="5"/>
+      <c r="G650" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H650" s="5">
+        <v>43172</v>
+      </c>
       <c r="I650" s="3"/>
       <c r="J650" s="3"/>
     </row>
     <row r="651" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A651" s="3"/>
-      <c r="B651" s="29"/>
-      <c r="C651" s="3"/>
-      <c r="D651" s="3"/>
-      <c r="E651" s="3"/>
+      <c r="A651" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B651" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C651" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D651" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E651" s="3">
+        <v>1</v>
+      </c>
       <c r="F651" s="3"/>
-      <c r="G651" s="3"/>
-      <c r="H651" s="5"/>
+      <c r="G651" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H651" s="5">
+        <v>43166</v>
+      </c>
       <c r="I651" s="3"/>
       <c r="J651" s="3"/>
     </row>
     <row r="652" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A652" s="3"/>
-      <c r="B652" s="29"/>
-      <c r="C652" s="3"/>
-      <c r="D652" s="3"/>
-      <c r="E652" s="3"/>
+      <c r="A652" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B652" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C652" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D652" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="E652" s="3">
+        <v>1</v>
+      </c>
       <c r="F652" s="3"/>
-      <c r="G652" s="3"/>
-      <c r="H652" s="5"/>
+      <c r="G652" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H652" s="5">
+        <v>43165</v>
+      </c>
       <c r="I652" s="3"/>
       <c r="J652" s="3"/>
     </row>
     <row r="653" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A653" s="3"/>
-      <c r="B653" s="29"/>
-      <c r="C653" s="3"/>
-      <c r="D653" s="3"/>
-      <c r="E653" s="3"/>
+      <c r="A653" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B653" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C653" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D653" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E653" s="3">
+        <v>1</v>
+      </c>
       <c r="F653" s="3"/>
-      <c r="G653" s="3"/>
-      <c r="H653" s="5"/>
+      <c r="G653" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H653" s="5">
+        <v>43165</v>
+      </c>
       <c r="I653" s="3"/>
       <c r="J653" s="3"/>
     </row>
     <row r="654" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A654" s="3"/>
-      <c r="B654" s="29"/>
-      <c r="C654" s="3"/>
-      <c r="D654" s="3"/>
-      <c r="E654" s="3"/>
+      <c r="A654" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B654" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C654" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D654" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E654" s="3">
+        <v>1</v>
+      </c>
       <c r="F654" s="3"/>
-      <c r="G654" s="3"/>
-      <c r="H654" s="5"/>
+      <c r="G654" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H654" s="5">
+        <v>43173</v>
+      </c>
       <c r="I654" s="3"/>
       <c r="J654" s="3"/>
     </row>
     <row r="655" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A655" s="3"/>
-      <c r="B655" s="29"/>
-      <c r="C655" s="3"/>
-      <c r="D655" s="3"/>
-      <c r="E655" s="3"/>
+      <c r="A655" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B655" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C655" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D655" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E655" s="3">
+        <v>1</v>
+      </c>
       <c r="F655" s="3"/>
-      <c r="G655" s="3"/>
-      <c r="H655" s="5"/>
+      <c r="G655" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H655" s="5">
+        <v>43173</v>
+      </c>
       <c r="I655" s="3"/>
       <c r="J655" s="3"/>
     </row>
     <row r="656" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A656" s="3"/>
-      <c r="B656" s="29"/>
-      <c r="C656" s="3"/>
-      <c r="D656" s="3"/>
-      <c r="E656" s="3"/>
+      <c r="A656" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B656" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C656" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D656" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E656" s="3">
+        <v>1</v>
+      </c>
       <c r="F656" s="3"/>
-      <c r="G656" s="3"/>
-      <c r="H656" s="5"/>
+      <c r="G656" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H656" s="5">
+        <v>43187</v>
+      </c>
       <c r="I656" s="3"/>
       <c r="J656" s="3"/>
     </row>
     <row r="657" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A657" s="3"/>
-      <c r="B657" s="29"/>
-      <c r="C657" s="3"/>
-      <c r="D657" s="3"/>
-      <c r="E657" s="3"/>
+      <c r="A657" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B657" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C657" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D657" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E657" s="3">
+        <v>1</v>
+      </c>
       <c r="F657" s="3"/>
-      <c r="G657" s="3"/>
-      <c r="H657" s="5"/>
+      <c r="G657" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H657" s="5">
+        <v>43173</v>
+      </c>
       <c r="I657" s="3"/>
       <c r="J657" s="3"/>
     </row>
     <row r="658" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A658" s="3"/>
-      <c r="B658" s="29"/>
-      <c r="C658" s="3"/>
-      <c r="D658" s="3"/>
-      <c r="E658" s="3"/>
+      <c r="A658" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B658" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C658" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D658" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E658" s="3">
+        <v>1</v>
+      </c>
       <c r="F658" s="3"/>
-      <c r="G658" s="3"/>
-      <c r="H658" s="5"/>
+      <c r="G658" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H658" s="5">
+        <v>43187</v>
+      </c>
       <c r="I658" s="3"/>
       <c r="J658" s="3"/>
     </row>
     <row r="659" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A659" s="3"/>
-      <c r="B659" s="29"/>
-      <c r="C659" s="3"/>
-      <c r="D659" s="3"/>
-      <c r="E659" s="3"/>
+      <c r="A659" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B659" s="40" t="s">
+        <v>377</v>
+      </c>
+      <c r="C659" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D659" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E659" s="3">
+        <v>2</v>
+      </c>
       <c r="F659" s="3"/>
-      <c r="G659" s="3"/>
-      <c r="H659" s="5"/>
+      <c r="G659" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H659" s="5">
+        <v>43179</v>
+      </c>
       <c r="I659" s="3"/>
       <c r="J659" s="3"/>
     </row>
     <row r="660" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A660" s="3"/>
-      <c r="B660" s="29"/>
-      <c r="C660" s="3"/>
-      <c r="D660" s="3"/>
-      <c r="E660" s="3"/>
+      <c r="A660" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B660" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C660" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D660" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E660" s="3">
+        <v>1</v>
+      </c>
       <c r="F660" s="3"/>
-      <c r="G660" s="3"/>
-      <c r="H660" s="5"/>
+      <c r="G660" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H660" s="5">
+        <v>43188</v>
+      </c>
       <c r="I660" s="3"/>
       <c r="J660" s="3"/>
     </row>
     <row r="661" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A661" s="3"/>
-      <c r="B661" s="29"/>
-      <c r="C661" s="3"/>
-      <c r="D661" s="3"/>
-      <c r="E661" s="3"/>
+      <c r="A661" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B661" s="40" t="s">
+        <v>375</v>
+      </c>
+      <c r="C661" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D661" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E661" s="3">
+        <v>1</v>
+      </c>
       <c r="F661" s="3"/>
-      <c r="G661" s="3"/>
-      <c r="H661" s="5"/>
-      <c r="I661" s="3"/>
+      <c r="G661" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H661" s="5">
+        <v>43188</v>
+      </c>
+      <c r="I661" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="J661" s="3"/>
     </row>
     <row r="662" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A662" s="3"/>
-      <c r="B662" s="29"/>
-      <c r="C662" s="3"/>
-      <c r="D662" s="3"/>
-      <c r="E662" s="3"/>
+      <c r="A662" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B662" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C662" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D662" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E662" s="3">
+        <v>1</v>
+      </c>
       <c r="F662" s="3"/>
-      <c r="G662" s="3"/>
-      <c r="H662" s="5"/>
+      <c r="G662" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H662" s="5">
+        <v>43185</v>
+      </c>
       <c r="I662" s="3"/>
       <c r="J662" s="3"/>
     </row>
     <row r="663" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A663" s="3"/>
-      <c r="B663" s="29"/>
-      <c r="C663" s="3"/>
-      <c r="D663" s="3"/>
-      <c r="E663" s="3"/>
+      <c r="A663" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B663" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="C663" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D663" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E663" s="3">
+        <v>1</v>
+      </c>
       <c r="F663" s="3"/>
-      <c r="G663" s="3"/>
-      <c r="H663" s="5"/>
+      <c r="G663" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H663" s="5">
+        <v>43185</v>
+      </c>
       <c r="I663" s="3"/>
       <c r="J663" s="3"/>
     </row>
     <row r="664" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A664" s="3"/>
-      <c r="B664" s="29"/>
-      <c r="C664" s="3"/>
-      <c r="D664" s="3"/>
-      <c r="E664" s="3"/>
+      <c r="A664" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B664" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="C664" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D664" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E664" s="3">
+        <v>1</v>
+      </c>
       <c r="F664" s="3"/>
-      <c r="G664" s="3"/>
-      <c r="H664" s="5"/>
+      <c r="G664" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H664" s="5">
+        <v>43186</v>
+      </c>
       <c r="I664" s="3"/>
       <c r="J664" s="3"/>
     </row>
     <row r="665" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A665" s="3"/>
-      <c r="B665" s="29"/>
-      <c r="C665" s="3"/>
-      <c r="D665" s="3"/>
-      <c r="E665" s="3"/>
-      <c r="F665" s="3"/>
-      <c r="G665" s="3"/>
-      <c r="H665" s="5"/>
-      <c r="I665" s="3"/>
-      <c r="J665" s="3"/>
+      <c r="A665" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B665" s="3">
+        <v>500.06</v>
+      </c>
+      <c r="C665" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D665" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E665" s="3">
+        <v>1</v>
+      </c>
+      <c r="F665" s="3">
+        <v>1</v>
+      </c>
+      <c r="G665" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H665" s="5">
+        <v>43186</v>
+      </c>
+      <c r="I665" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J665" s="3" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="666" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A666" s="3"/>
-      <c r="B666" s="29"/>
-      <c r="C666" s="3"/>
-      <c r="D666" s="3"/>
-      <c r="E666" s="3"/>
+      <c r="A666" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B666" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="C666" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D666" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E666" s="3">
+        <v>1</v>
+      </c>
       <c r="F666" s="3"/>
-      <c r="G666" s="3"/>
-      <c r="H666" s="5"/>
+      <c r="G666" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H666" s="5">
+        <v>43172</v>
+      </c>
       <c r="I666" s="3"/>
       <c r="J666" s="3"/>
     </row>
     <row r="667" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A667" s="3"/>
-      <c r="B667" s="29"/>
-      <c r="C667" s="3"/>
-      <c r="D667" s="3"/>
-      <c r="E667" s="3"/>
+      <c r="A667" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B667" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="C667" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D667" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E667" s="3">
+        <v>1</v>
+      </c>
       <c r="F667" s="3"/>
-      <c r="G667" s="3"/>
-      <c r="H667" s="5"/>
+      <c r="G667" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H667" s="5">
+        <v>43187</v>
+      </c>
       <c r="I667" s="3"/>
       <c r="J667" s="3"/>
     </row>
     <row r="668" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A668" s="3"/>
-      <c r="B668" s="29"/>
-      <c r="C668" s="3"/>
-      <c r="D668" s="3"/>
-      <c r="E668" s="3"/>
+      <c r="A668" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B668" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="C668" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D668" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E668" s="3">
+        <v>1</v>
+      </c>
       <c r="F668" s="3"/>
-      <c r="G668" s="3"/>
-      <c r="H668" s="5"/>
-      <c r="I668" s="3"/>
-      <c r="J668" s="3"/>
+      <c r="G668" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H668" s="5">
+        <v>43188</v>
+      </c>
+      <c r="I668" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J668" s="3" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="669" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A669" s="3"/>
-      <c r="B669" s="29"/>
-      <c r="C669" s="3"/>
-      <c r="D669" s="3"/>
-      <c r="E669" s="3"/>
+      <c r="A669" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B669" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="C669" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D669" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E669" s="3">
+        <v>1</v>
+      </c>
       <c r="F669" s="3"/>
-      <c r="G669" s="3"/>
-      <c r="H669" s="5"/>
-      <c r="I669" s="3"/>
-      <c r="J669" s="3"/>
+      <c r="G669" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H669" s="5">
+        <v>43188</v>
+      </c>
+      <c r="I669" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J669" s="3" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="670" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A670" s="3"/>
-      <c r="B670" s="29"/>
-      <c r="C670" s="3"/>
-      <c r="D670" s="3"/>
-      <c r="E670" s="3"/>
+      <c r="A670" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B670" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="C670" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D670" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E670" s="3">
+        <v>1</v>
+      </c>
       <c r="F670" s="3"/>
-      <c r="G670" s="3"/>
-      <c r="H670" s="5"/>
+      <c r="G670" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H670" s="5">
+        <v>43189</v>
+      </c>
       <c r="I670" s="3"/>
       <c r="J670" s="3"/>
     </row>
@@ -27837,60 +29266,80 @@
       <c r="I1366" s="3"/>
       <c r="J1366" s="3"/>
     </row>
-    <row r="1367" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1367" s="3"/>
-      <c r="B1367" s="29"/>
-      <c r="C1367" s="3"/>
-      <c r="D1367" s="3"/>
-      <c r="E1367" s="3"/>
-      <c r="F1367" s="3"/>
-      <c r="G1367" s="3"/>
-      <c r="H1367" s="5"/>
-      <c r="I1367" s="3"/>
-      <c r="J1367" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J587"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B615 B589:B614 B641 B623" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>SQA!$A$1:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>A1:A1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Reasons for Disapproval'!$A$1:$A$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>I1:I1048576</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'A or D'!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G315 G317:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Application!$A$2:$A$49</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Deliverable Types'!$A$1:$A$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>G2:G315 G317:G661 G671:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 282018.xlsx]A or D'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G316</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>SQA!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A661 A671:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Reasons for Disapproval'!$A$1:$A$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>I1:I661 I671:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Application!$A$2:$A$49</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1363:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Deliverable Types'!$A$1:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D661 D671:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Nick First Pass Acceptance.xlsx]Deliverable Types'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D662:D670</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Application!$A$2:$A$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C1362</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Nick First Pass Acceptance.xlsx]A or D'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>G662:G670</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Nick First Pass Acceptance.xlsx]Reasons for Disapproval'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>I662:I670</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[Nick First Pass Acceptance.xlsx]SQA'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>A662:A670</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -27935,10 +29384,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A49"/>
+  <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A50" sqref="A2:A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28143,57 +29592,62 @@
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>450</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>378</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>47</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A49">
-    <sortCondition ref="A2:A49"/>
+  <sortState ref="A2:A50">
+    <sortCondition ref="A2:A50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
EOD and End of ACR
</commit_message>
<xml_diff>
--- a/data/First Pass Acceptance.xlsx
+++ b/data/First Pass Acceptance.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\firstPassAcceptance\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{60D0F35F-7188-4218-8CBD-747E5C1656B4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11445" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11445" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACR" sheetId="7" r:id="rId1"/>
@@ -28,6 +29,7 @@
     <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ACR!$A$1:$J$119</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Application!$A$1:$A$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FPA!$A$1:$J$1385</definedName>
   </definedNames>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12485" uniqueCount="1176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12757" uniqueCount="1222">
   <si>
     <t>Project ID</t>
   </si>
@@ -3579,11 +3581,149 @@
   <si>
     <t>1003</t>
   </si>
+  <si>
+    <t>OE fials to show what the region was changed to.</t>
+  </si>
+  <si>
+    <t>18-37191</t>
+  </si>
+  <si>
+    <t>18-36471</t>
+  </si>
+  <si>
+    <t>CSIT09308</t>
+  </si>
+  <si>
+    <t>CSIT09307</t>
+  </si>
+  <si>
+    <t>CSIT09311</t>
+  </si>
+  <si>
+    <t>CSIT09310</t>
+  </si>
+  <si>
+    <t>CSIT09309</t>
+  </si>
+  <si>
+    <t>CSIT09314</t>
+  </si>
+  <si>
+    <t>Iclude before OE is non-compliant and incomplete</t>
+  </si>
+  <si>
+    <t>18-37352</t>
+  </si>
+  <si>
+    <t>18-37351</t>
+  </si>
+  <si>
+    <t>18-37549</t>
+  </si>
+  <si>
+    <t>18-37718</t>
+  </si>
+  <si>
+    <t>18-37980</t>
+  </si>
+  <si>
+    <t>CSIT09316</t>
+  </si>
+  <si>
+    <t>CSIT09188</t>
+  </si>
+  <si>
+    <t>CSIT09288</t>
+  </si>
+  <si>
+    <t>CSIT09301</t>
+  </si>
+  <si>
+    <t>CSIT09319</t>
+  </si>
+  <si>
+    <t>CSIT09318</t>
+  </si>
+  <si>
+    <t>CSIT09325</t>
+  </si>
+  <si>
+    <t>CSIT09324</t>
+  </si>
+  <si>
+    <t>CSIT09322</t>
+  </si>
+  <si>
+    <t>CSIT09321</t>
+  </si>
+  <si>
+    <t>CSIT09320</t>
+  </si>
+  <si>
+    <t>CSIT09317</t>
+  </si>
+  <si>
+    <t>CSIT09327</t>
+  </si>
+  <si>
+    <t>CSIT09333</t>
+  </si>
+  <si>
+    <t>CSIT09332</t>
+  </si>
+  <si>
+    <t>CSIT09329</t>
+  </si>
+  <si>
+    <t>CSIT09335</t>
+  </si>
+  <si>
+    <t>CSIT09340</t>
+  </si>
+  <si>
+    <t>CSIT09341</t>
+  </si>
+  <si>
+    <t>CSIT09346</t>
+  </si>
+  <si>
+    <t>CSIT09344</t>
+  </si>
+  <si>
+    <t>CSIT09328</t>
+  </si>
+  <si>
+    <t>CSIT09339</t>
+  </si>
+  <si>
+    <t>CSIT09345</t>
+  </si>
+  <si>
+    <t>CSIT09350</t>
+  </si>
+  <si>
+    <t>CSIT09147</t>
+  </si>
+  <si>
+    <t>Change not made to some items</t>
+  </si>
+  <si>
+    <t>CSIT09144</t>
+  </si>
+  <si>
+    <t>CSIT09175</t>
+  </si>
+  <si>
+    <t>CSIT09174</t>
+  </si>
+  <si>
+    <t>CSIT09277</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -4291,12 +4431,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E73" sqref="E73"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4345,22 +4485,25 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>779</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>1044</v>
+        <v>1052</v>
       </c>
       <c r="D2" s="47">
-        <v>43376</v>
+        <v>43385</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
       </c>
       <c r="F2" t="s">
-        <v>1097</v>
+        <v>1052</v>
       </c>
       <c r="G2" s="47">
-        <v>43383</v>
+        <v>43411</v>
       </c>
       <c r="H2" t="s">
         <v>74</v>
@@ -4368,174 +4511,120 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>779</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>1045</v>
+        <v>1053</v>
       </c>
       <c r="D3" s="47">
-        <v>43376</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1098</v>
-      </c>
-      <c r="G3" s="47">
-        <v>43376</v>
-      </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1112</v>
+        <v>43390</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>779</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>1045</v>
+        <v>1055</v>
       </c>
       <c r="D4" s="47">
-        <v>43376</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1098</v>
-      </c>
-      <c r="G4" s="47">
-        <v>43376</v>
-      </c>
-      <c r="H4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1113</v>
+        <v>43403</v>
+      </c>
+      <c r="E4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>779</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>1045</v>
+        <v>1122</v>
       </c>
       <c r="D5" s="47">
-        <v>43376</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1098</v>
-      </c>
-      <c r="G5" s="47">
-        <v>43376</v>
-      </c>
-      <c r="H5" t="s">
-        <v>57</v>
+        <v>43423</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>779</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>316</v>
       </c>
       <c r="C6" t="s">
-        <v>1046</v>
+        <v>1126</v>
       </c>
       <c r="D6" s="47">
-        <v>43376</v>
-      </c>
-      <c r="F6" t="s">
-        <v>1099</v>
-      </c>
-      <c r="G6" s="47">
-        <v>43376</v>
-      </c>
-      <c r="H6" t="s">
+        <v>43424</v>
+      </c>
+      <c r="E6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>779</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>316</v>
       </c>
       <c r="C7" t="s">
-        <v>1047</v>
+        <v>1127</v>
       </c>
       <c r="D7" s="47">
-        <v>43375</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1100</v>
-      </c>
-      <c r="G7" s="47">
-        <v>43376</v>
-      </c>
-      <c r="H7" t="s">
+        <v>43423</v>
+      </c>
+      <c r="E7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>779</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>316</v>
       </c>
       <c r="C8" t="s">
-        <v>1048</v>
+        <v>1128</v>
       </c>
       <c r="D8" s="47">
-        <v>43375</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1101</v>
-      </c>
-      <c r="G8" s="47">
-        <v>43376</v>
-      </c>
-      <c r="H8" t="s">
+        <v>43420</v>
+      </c>
+      <c r="E8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>779</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>1129</v>
       </c>
       <c r="C9" t="s">
-        <v>1049</v>
+        <v>1130</v>
       </c>
       <c r="D9" s="47">
-        <v>43375</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1102</v>
-      </c>
-      <c r="G9" s="47">
-        <v>43376</v>
-      </c>
-      <c r="H9" t="s">
+        <v>43430</v>
+      </c>
+      <c r="E9" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4547,16 +4636,16 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>1050</v>
+        <v>1044</v>
       </c>
       <c r="D10" s="47">
-        <v>43375</v>
+        <v>43376</v>
       </c>
       <c r="F10" t="s">
-        <v>1103</v>
+        <v>1097</v>
       </c>
       <c r="G10" s="47">
-        <v>43376</v>
+        <v>43383</v>
       </c>
       <c r="H10" t="s">
         <v>74</v>
@@ -4570,62 +4659,77 @@
         <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>1051</v>
+        <v>1045</v>
       </c>
       <c r="D11" s="47">
-        <v>43370</v>
+        <v>43376</v>
       </c>
       <c r="F11" t="s">
-        <v>1104</v>
+        <v>1098</v>
       </c>
       <c r="G11" s="47">
-        <v>43381</v>
+        <v>43376</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>58</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1112</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>779</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>1052</v>
+        <v>1045</v>
       </c>
       <c r="D12" s="47">
-        <v>43385</v>
-      </c>
-      <c r="E12" t="s">
-        <v>74</v>
+        <v>43376</v>
       </c>
       <c r="F12" t="s">
-        <v>1052</v>
+        <v>1098</v>
       </c>
       <c r="G12" s="47">
-        <v>43411</v>
+        <v>43376</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>58</v>
+      </c>
+      <c r="I12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1113</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>779</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>1053</v>
+        <v>1045</v>
       </c>
       <c r="D13" s="47">
-        <v>43390</v>
-      </c>
-      <c r="E13" t="s">
-        <v>74</v>
+        <v>43376</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G13" s="47">
+        <v>43376</v>
+      </c>
+      <c r="H13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -4636,16 +4740,16 @@
         <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>1054</v>
+        <v>1046</v>
       </c>
       <c r="D14" s="47">
-        <v>43403</v>
+        <v>43376</v>
       </c>
       <c r="F14" t="s">
-        <v>1105</v>
+        <v>1099</v>
       </c>
       <c r="G14" s="47">
-        <v>43403</v>
+        <v>43376</v>
       </c>
       <c r="H14" t="s">
         <v>74</v>
@@ -4653,378 +4757,429 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>779</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>1055</v>
+        <v>1047</v>
       </c>
       <c r="D15" s="47">
-        <v>43403</v>
-      </c>
-      <c r="E15" t="s">
+        <v>43375</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1100</v>
+      </c>
+      <c r="G15" s="47">
+        <v>43376</v>
+      </c>
+      <c r="H15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>1056</v>
+        <v>1048</v>
       </c>
       <c r="D16" s="47">
-        <v>43374</v>
+        <v>43375</v>
       </c>
       <c r="F16" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1101</v>
+      </c>
+      <c r="G16" s="47">
+        <v>43376</v>
+      </c>
+      <c r="H16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>1057</v>
+        <v>1049</v>
       </c>
       <c r="D17" s="47">
-        <v>43363</v>
+        <v>43375</v>
       </c>
       <c r="F17" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="G17" s="47">
         <v>43376</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>1058</v>
+        <v>1050</v>
       </c>
       <c r="D18" s="47">
+        <v>43375</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G18" s="47">
         <v>43376</v>
       </c>
-      <c r="F18" t="s">
-        <v>1058</v>
-      </c>
-      <c r="G18" s="47">
-        <v>43377</v>
-      </c>
       <c r="H18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>1059</v>
+        <v>1051</v>
       </c>
       <c r="D19" s="47">
-        <v>42818</v>
+        <v>43370</v>
       </c>
       <c r="F19" t="s">
-        <v>1059</v>
+        <v>1104</v>
       </c>
       <c r="G19" s="47">
-        <v>43376</v>
+        <v>43381</v>
       </c>
       <c r="H19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>1060</v>
+        <v>1054</v>
       </c>
       <c r="D20" s="47">
-        <v>43369</v>
+        <v>43403</v>
       </c>
       <c r="F20" t="s">
-        <v>1060</v>
+        <v>1105</v>
       </c>
       <c r="G20" s="47">
-        <v>43376</v>
+        <v>43403</v>
       </c>
       <c r="H20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>1061</v>
+        <v>1133</v>
       </c>
       <c r="D21" s="47">
-        <v>43356</v>
+        <v>43419</v>
+      </c>
+      <c r="E21" t="s">
+        <v>74</v>
       </c>
       <c r="F21" t="s">
-        <v>1107</v>
+        <v>1134</v>
       </c>
       <c r="G21" s="47">
-        <v>43377</v>
+        <v>43430</v>
       </c>
       <c r="H21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>1062</v>
+        <v>1135</v>
       </c>
       <c r="D22" s="47">
-        <v>43280</v>
+        <v>43419</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
       </c>
       <c r="F22" t="s">
-        <v>1062</v>
+        <v>1136</v>
       </c>
       <c r="G22" s="47">
-        <v>43377</v>
+        <v>43430</v>
       </c>
       <c r="H22" t="s">
-        <v>57</v>
-      </c>
-      <c r="J22" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>1063</v>
+        <v>1137</v>
       </c>
       <c r="D23" s="47">
-        <v>43290</v>
+        <v>43430</v>
+      </c>
+      <c r="E23" t="s">
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>1063</v>
+        <v>1138</v>
       </c>
       <c r="G23" s="47">
-        <v>43377</v>
+        <v>43433</v>
       </c>
       <c r="H23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>1064</v>
+        <v>1139</v>
       </c>
       <c r="D24" s="47">
-        <v>43370</v>
+        <v>43418</v>
+      </c>
+      <c r="E24" t="s">
+        <v>74</v>
       </c>
       <c r="F24" t="s">
-        <v>1064</v>
+        <v>1140</v>
       </c>
       <c r="G24" s="47">
-        <v>43377</v>
+        <v>43430</v>
       </c>
       <c r="H24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>1065</v>
+        <v>1141</v>
       </c>
       <c r="D25" s="47">
-        <v>43377</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>43417</v>
+      </c>
+      <c r="E25" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G25" s="47">
+        <v>43430</v>
+      </c>
+      <c r="H25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>1066</v>
+        <v>1143</v>
       </c>
       <c r="D26" s="47">
-        <v>43377</v>
+        <v>43419</v>
+      </c>
+      <c r="E26" t="s">
+        <v>74</v>
       </c>
       <c r="F26" t="s">
-        <v>1066</v>
+        <v>1144</v>
       </c>
       <c r="G26" s="47">
-        <v>43389</v>
+        <v>43430</v>
       </c>
       <c r="H26" t="s">
-        <v>57</v>
-      </c>
-      <c r="J26" t="s">
-        <v>1114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>1067</v>
+        <v>1145</v>
       </c>
       <c r="D27" s="47">
-        <v>43031</v>
+        <v>43419</v>
+      </c>
+      <c r="E27" t="s">
+        <v>74</v>
       </c>
       <c r="F27" t="s">
-        <v>1067</v>
+        <v>1146</v>
       </c>
       <c r="G27" s="47">
-        <v>43377</v>
+        <v>43430</v>
       </c>
       <c r="H27" t="s">
-        <v>57</v>
-      </c>
-      <c r="J27" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B28" t="s">
-        <v>912</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>1068</v>
+        <v>1147</v>
       </c>
       <c r="D28" s="47">
-        <v>43378</v>
+        <v>43430</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
       </c>
       <c r="F28" t="s">
-        <v>1108</v>
+        <v>1148</v>
       </c>
       <c r="G28" s="47">
-        <v>43389</v>
+        <v>43434</v>
       </c>
       <c r="H28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>1069</v>
+        <v>1149</v>
       </c>
       <c r="D29" s="47">
-        <v>43381</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>43430</v>
+      </c>
+      <c r="E29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G29" s="47">
+        <v>43434</v>
+      </c>
+      <c r="H29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>1070</v>
+        <v>1150</v>
       </c>
       <c r="D30" s="47">
-        <v>42704</v>
+        <v>43430</v>
+      </c>
+      <c r="E30" t="s">
+        <v>74</v>
       </c>
       <c r="F30" t="s">
-        <v>1070</v>
+        <v>1138</v>
       </c>
       <c r="G30" s="47">
-        <v>43381</v>
+        <v>43433</v>
       </c>
       <c r="H30" t="s">
-        <v>57</v>
-      </c>
-      <c r="J30" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>779</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>1071</v>
+        <v>1151</v>
       </c>
       <c r="D31" s="47">
-        <v>42597</v>
+        <v>43433</v>
+      </c>
+      <c r="E31" t="s">
+        <v>74</v>
       </c>
       <c r="F31" t="s">
-        <v>1071</v>
+        <v>1152</v>
       </c>
       <c r="G31" s="47">
-        <v>43381</v>
+        <v>43434</v>
       </c>
       <c r="H31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -5032,19 +5187,16 @@
         <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>1072</v>
+        <v>1056</v>
       </c>
       <c r="D32" s="47">
-        <v>43360</v>
+        <v>43374</v>
+      </c>
+      <c r="E32" t="s">
+        <v>57</v>
       </c>
       <c r="F32" t="s">
-        <v>1072</v>
-      </c>
-      <c r="G32" s="47">
-        <v>43381</v>
-      </c>
-      <c r="H32" t="s">
-        <v>57</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -5055,19 +5207,22 @@
         <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>1073</v>
+        <v>1057</v>
       </c>
       <c r="D33" s="47">
-        <v>43384</v>
+        <v>43363</v>
+      </c>
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1106</v>
+      </c>
+      <c r="G33" s="47">
+        <v>43376</v>
       </c>
       <c r="H33" t="s">
-        <v>58</v>
-      </c>
-      <c r="I33" t="s">
-        <v>31</v>
-      </c>
-      <c r="J33" t="s">
-        <v>1115</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -5075,22 +5230,25 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>1073</v>
+        <v>1058</v>
       </c>
       <c r="D34" s="47">
-        <v>43385</v>
+        <v>43376</v>
+      </c>
+      <c r="E34" t="s">
+        <v>57</v>
       </c>
       <c r="F34" t="s">
-        <v>1109</v>
+        <v>1058</v>
       </c>
       <c r="G34" s="47">
-        <v>43389</v>
+        <v>43377</v>
       </c>
       <c r="H34" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -5101,16 +5259,19 @@
         <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>1074</v>
+        <v>1059</v>
       </c>
       <c r="D35" s="47">
-        <v>43389</v>
+        <v>42818</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
       </c>
       <c r="F35" t="s">
-        <v>1074</v>
+        <v>1059</v>
       </c>
       <c r="G35" s="47">
-        <v>43398</v>
+        <v>43376</v>
       </c>
       <c r="H35" t="s">
         <v>57</v>
@@ -5124,16 +5285,19 @@
         <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>1075</v>
+        <v>1060</v>
       </c>
       <c r="D36" s="47">
-        <v>43250</v>
+        <v>43369</v>
+      </c>
+      <c r="E36" t="s">
+        <v>57</v>
       </c>
       <c r="F36" t="s">
-        <v>1075</v>
+        <v>1060</v>
       </c>
       <c r="G36" s="47">
-        <v>43389</v>
+        <v>43376</v>
       </c>
       <c r="H36" t="s">
         <v>57</v>
@@ -5144,19 +5308,22 @@
         <v>39</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C37" t="s">
-        <v>1076</v>
+        <v>1061</v>
       </c>
       <c r="D37" s="47">
-        <v>43223</v>
+        <v>43356</v>
+      </c>
+      <c r="E37" t="s">
+        <v>57</v>
       </c>
       <c r="F37" t="s">
-        <v>1076</v>
+        <v>1107</v>
       </c>
       <c r="G37" s="47">
-        <v>43389</v>
+        <v>43377</v>
       </c>
       <c r="H37" t="s">
         <v>57</v>
@@ -5170,20 +5337,26 @@
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>1077</v>
+        <v>1062</v>
       </c>
       <c r="D38" s="47">
-        <v>43223</v>
+        <v>43280</v>
+      </c>
+      <c r="E38" t="s">
+        <v>57</v>
       </c>
       <c r="F38" t="s">
-        <v>1077</v>
+        <v>1062</v>
       </c>
       <c r="G38" s="47">
-        <v>43389</v>
+        <v>43377</v>
       </c>
       <c r="H38" t="s">
         <v>57</v>
       </c>
+      <c r="J38" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -5193,16 +5366,19 @@
         <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>1078</v>
+        <v>1063</v>
       </c>
       <c r="D39" s="47">
-        <v>43287</v>
+        <v>43290</v>
+      </c>
+      <c r="E39" t="s">
+        <v>57</v>
       </c>
       <c r="F39" t="s">
-        <v>1078</v>
+        <v>1063</v>
       </c>
       <c r="G39" s="47">
-        <v>43389</v>
+        <v>43377</v>
       </c>
       <c r="H39" t="s">
         <v>57</v>
@@ -5216,16 +5392,19 @@
         <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="D40" s="47">
-        <v>43298</v>
+        <v>43370</v>
+      </c>
+      <c r="E40" t="s">
+        <v>57</v>
       </c>
       <c r="F40" t="s">
-        <v>1079</v>
+        <v>1064</v>
       </c>
       <c r="G40" s="47">
-        <v>43389</v>
+        <v>43377</v>
       </c>
       <c r="H40" t="s">
         <v>57</v>
@@ -5236,21 +5415,15 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>1080</v>
+        <v>1065</v>
       </c>
       <c r="D41" s="47">
-        <v>43339</v>
-      </c>
-      <c r="F41" t="s">
-        <v>1080</v>
-      </c>
-      <c r="G41" s="47">
-        <v>43389</v>
-      </c>
-      <c r="H41" t="s">
+        <v>43377</v>
+      </c>
+      <c r="E41" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5262,13 +5435,16 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>1081</v>
+        <v>1066</v>
       </c>
       <c r="D42" s="47">
-        <v>43367</v>
+        <v>43377</v>
+      </c>
+      <c r="E42" t="s">
+        <v>57</v>
       </c>
       <c r="F42" t="s">
-        <v>1081</v>
+        <v>1066</v>
       </c>
       <c r="G42" s="47">
         <v>43389</v>
@@ -5276,6 +5452,9 @@
       <c r="H42" t="s">
         <v>57</v>
       </c>
+      <c r="J42" t="s">
+        <v>1114</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -5285,36 +5464,45 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>1082</v>
+        <v>1067</v>
       </c>
       <c r="D43" s="47">
-        <v>43354</v>
+        <v>43031</v>
+      </c>
+      <c r="E43" t="s">
+        <v>57</v>
       </c>
       <c r="F43" t="s">
-        <v>1082</v>
+        <v>1067</v>
       </c>
       <c r="G43" s="47">
-        <v>43389</v>
+        <v>43377</v>
       </c>
       <c r="H43" t="s">
         <v>57</v>
       </c>
+      <c r="J43" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>912</v>
       </c>
       <c r="C44" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="D44" s="47">
-        <v>43360</v>
+        <v>43378</v>
+      </c>
+      <c r="E44" t="s">
+        <v>57</v>
       </c>
       <c r="F44" t="s">
-        <v>1072</v>
+        <v>1108</v>
       </c>
       <c r="G44" s="47">
         <v>43389</v>
@@ -5328,21 +5516,15 @@
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>1083</v>
+        <v>1069</v>
       </c>
       <c r="D45" s="47">
-        <v>43363</v>
-      </c>
-      <c r="F45" t="s">
-        <v>1083</v>
-      </c>
-      <c r="G45" s="47">
-        <v>43389</v>
-      </c>
-      <c r="H45" t="s">
+        <v>43381</v>
+      </c>
+      <c r="E45" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5354,25 +5536,25 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>1084</v>
+        <v>1070</v>
       </c>
       <c r="D46" s="47">
-        <v>43384</v>
+        <v>42704</v>
+      </c>
+      <c r="E46" t="s">
+        <v>57</v>
       </c>
       <c r="F46" t="s">
-        <v>1084</v>
+        <v>1070</v>
       </c>
       <c r="G46" s="47">
-        <v>43396</v>
+        <v>43381</v>
       </c>
       <c r="H46" t="s">
         <v>57</v>
       </c>
-      <c r="I46" t="s">
-        <v>36</v>
-      </c>
       <c r="J46" t="s">
-        <v>1116</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -5383,16 +5565,19 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>1085</v>
+        <v>1071</v>
       </c>
       <c r="D47" s="47">
-        <v>43384</v>
+        <v>42597</v>
+      </c>
+      <c r="E47" t="s">
+        <v>57</v>
       </c>
       <c r="F47" t="s">
-        <v>1085</v>
+        <v>1071</v>
       </c>
       <c r="G47" s="47">
-        <v>43389</v>
+        <v>43381</v>
       </c>
       <c r="H47" t="s">
         <v>57</v>
@@ -5403,13 +5588,25 @@
         <v>39</v>
       </c>
       <c r="B48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>1086</v>
+        <v>1072</v>
       </c>
       <c r="D48" s="47">
-        <v>43391</v>
+        <v>43360</v>
+      </c>
+      <c r="E48" t="s">
+        <v>57</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G48" s="47">
+        <v>43381</v>
+      </c>
+      <c r="H48" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -5417,22 +5614,22 @@
         <v>39</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>1087</v>
+        <v>1073</v>
       </c>
       <c r="D49" s="47">
-        <v>43391</v>
-      </c>
-      <c r="F49" t="s">
-        <v>1087</v>
-      </c>
-      <c r="G49" s="47">
-        <v>43396</v>
-      </c>
-      <c r="H49" t="s">
-        <v>57</v>
+        <v>43384</v>
+      </c>
+      <c r="E49" t="s">
+        <v>58</v>
+      </c>
+      <c r="I49" t="s">
+        <v>31</v>
+      </c>
+      <c r="J49" t="s">
+        <v>1115</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -5440,25 +5637,25 @@
         <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C50" t="s">
-        <v>1088</v>
+        <v>1073</v>
       </c>
       <c r="D50" s="47">
-        <v>43301</v>
+        <v>43385</v>
+      </c>
+      <c r="E50" t="s">
+        <v>57</v>
       </c>
       <c r="F50" t="s">
-        <v>1088</v>
+        <v>1109</v>
       </c>
       <c r="G50" s="47">
-        <v>43396</v>
+        <v>43389</v>
       </c>
       <c r="H50" t="s">
-        <v>57</v>
-      </c>
-      <c r="J50">
-        <v>43391</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -5469,16 +5666,19 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>1089</v>
+        <v>1074</v>
       </c>
       <c r="D51" s="47">
-        <v>43392</v>
+        <v>43389</v>
+      </c>
+      <c r="E51" t="s">
+        <v>57</v>
       </c>
       <c r="F51" t="s">
-        <v>1089</v>
+        <v>1074</v>
       </c>
       <c r="G51" s="47">
-        <v>43396</v>
+        <v>43398</v>
       </c>
       <c r="H51" t="s">
         <v>57</v>
@@ -5492,10 +5692,22 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>1090</v>
+        <v>1075</v>
       </c>
       <c r="D52" s="47">
-        <v>43396</v>
+        <v>43250</v>
+      </c>
+      <c r="E52" t="s">
+        <v>57</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G52" s="47">
+        <v>43389</v>
+      </c>
+      <c r="H52" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -5506,16 +5718,19 @@
         <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>1091</v>
+        <v>1076</v>
       </c>
       <c r="D53" s="47">
-        <v>43396</v>
+        <v>43223</v>
+      </c>
+      <c r="E53" t="s">
+        <v>57</v>
       </c>
       <c r="F53" t="s">
-        <v>1091</v>
+        <v>1076</v>
       </c>
       <c r="G53" s="47">
-        <v>43398</v>
+        <v>43389</v>
       </c>
       <c r="H53" t="s">
         <v>57</v>
@@ -5526,19 +5741,22 @@
         <v>39</v>
       </c>
       <c r="B54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>1092</v>
+        <v>1077</v>
       </c>
       <c r="D54" s="47">
-        <v>43397</v>
+        <v>43223</v>
+      </c>
+      <c r="E54" t="s">
+        <v>57</v>
       </c>
       <c r="F54" t="s">
-        <v>1110</v>
+        <v>1077</v>
       </c>
       <c r="G54" s="47">
-        <v>43397</v>
+        <v>43389</v>
       </c>
       <c r="H54" t="s">
         <v>57</v>
@@ -5552,10 +5770,22 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>1093</v>
+        <v>1078</v>
       </c>
       <c r="D55" s="47">
-        <v>43398</v>
+        <v>43287</v>
+      </c>
+      <c r="E55" t="s">
+        <v>57</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1078</v>
+      </c>
+      <c r="G55" s="47">
+        <v>43389</v>
+      </c>
+      <c r="H55" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -5566,10 +5796,22 @@
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>1094</v>
+        <v>1079</v>
       </c>
       <c r="D56" s="47">
-        <v>43403</v>
+        <v>43298</v>
+      </c>
+      <c r="E56" t="s">
+        <v>57</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G56" s="47">
+        <v>43389</v>
+      </c>
+      <c r="H56" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -5577,19 +5819,25 @@
         <v>39</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>1095</v>
+        <v>1080</v>
       </c>
       <c r="D57" s="47">
-        <v>43403</v>
+        <v>43339</v>
+      </c>
+      <c r="E57" t="s">
+        <v>57</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G57" s="47">
+        <v>43389</v>
       </c>
       <c r="H57" t="s">
-        <v>58</v>
-      </c>
-      <c r="I57" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -5597,19 +5845,22 @@
         <v>39</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>1096</v>
+        <v>1081</v>
       </c>
       <c r="D58" s="47">
-        <v>43398</v>
+        <v>43367</v>
+      </c>
+      <c r="E58" t="s">
+        <v>57</v>
       </c>
       <c r="F58" t="s">
-        <v>1111</v>
+        <v>1081</v>
       </c>
       <c r="G58" s="47">
-        <v>43404</v>
+        <v>43389</v>
       </c>
       <c r="H58" t="s">
         <v>57</v>
@@ -5617,399 +5868,1401 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C59" t="s">
-        <v>1122</v>
+        <v>1082</v>
       </c>
       <c r="D59" s="47">
-        <v>43423</v>
+        <v>43354</v>
       </c>
       <c r="E59" t="s">
-        <v>74</v>
+        <v>57</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1082</v>
+      </c>
+      <c r="G59" s="47">
+        <v>43389</v>
+      </c>
+      <c r="H59" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B60" t="s">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="C60" t="s">
-        <v>1126</v>
+        <v>1072</v>
       </c>
       <c r="D60" s="47">
-        <v>43424</v>
+        <v>43360</v>
       </c>
       <c r="E60" t="s">
-        <v>74</v>
+        <v>57</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G60" s="47">
+        <v>43389</v>
+      </c>
+      <c r="H60" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
-        <v>1127</v>
+        <v>1083</v>
       </c>
       <c r="D61" s="47">
-        <v>43423</v>
+        <v>43363</v>
       </c>
       <c r="E61" t="s">
-        <v>74</v>
+        <v>57</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1083</v>
+      </c>
+      <c r="G61" s="47">
+        <v>43389</v>
+      </c>
+      <c r="H61" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B62" t="s">
-        <v>316</v>
+        <v>45</v>
       </c>
       <c r="C62" t="s">
-        <v>1128</v>
+        <v>1084</v>
       </c>
       <c r="D62" s="47">
-        <v>43420</v>
+        <v>43384</v>
       </c>
       <c r="E62" t="s">
-        <v>74</v>
+        <v>57</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1084</v>
+      </c>
+      <c r="G62" s="47">
+        <v>43396</v>
+      </c>
+      <c r="H62" t="s">
+        <v>57</v>
+      </c>
+      <c r="I62" t="s">
+        <v>36</v>
+      </c>
+      <c r="J62" t="s">
+        <v>1116</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B63" t="s">
-        <v>1129</v>
+        <v>45</v>
       </c>
       <c r="C63" t="s">
-        <v>1130</v>
+        <v>1085</v>
       </c>
       <c r="D63" s="47">
-        <v>43430</v>
+        <v>43384</v>
       </c>
       <c r="E63" t="s">
-        <v>74</v>
+        <v>57</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1085</v>
+      </c>
+      <c r="G63" s="47">
+        <v>43389</v>
+      </c>
+      <c r="H63" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>779</v>
+        <v>39</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C64" t="s">
-        <v>1133</v>
+        <v>1086</v>
       </c>
       <c r="D64" s="47">
+        <v>43391</v>
+      </c>
+      <c r="E64" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D65" s="47">
+        <v>43391</v>
+      </c>
+      <c r="E65" t="s">
+        <v>57</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G65" s="47">
+        <v>43396</v>
+      </c>
+      <c r="H65" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1088</v>
+      </c>
+      <c r="D66" s="47">
+        <v>43301</v>
+      </c>
+      <c r="E66" t="s">
+        <v>57</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1088</v>
+      </c>
+      <c r="G66" s="47">
+        <v>43396</v>
+      </c>
+      <c r="H66" t="s">
+        <v>57</v>
+      </c>
+      <c r="J66">
+        <v>43391</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" t="s">
+        <v>45</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D67" s="47">
+        <v>43392</v>
+      </c>
+      <c r="E67" t="s">
+        <v>57</v>
+      </c>
+      <c r="F67" t="s">
+        <v>1089</v>
+      </c>
+      <c r="G67" s="47">
+        <v>43396</v>
+      </c>
+      <c r="H67" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>39</v>
+      </c>
+      <c r="B68" t="s">
+        <v>45</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D68" s="47">
+        <v>43396</v>
+      </c>
+      <c r="E68" t="s">
+        <v>57</v>
+      </c>
+      <c r="F68" t="s">
+        <v>1090</v>
+      </c>
+      <c r="G68" s="47">
+        <v>43418</v>
+      </c>
+      <c r="H68" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>39</v>
+      </c>
+      <c r="B69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D69" s="47">
+        <v>43396</v>
+      </c>
+      <c r="E69" t="s">
+        <v>57</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G69" s="47">
+        <v>43398</v>
+      </c>
+      <c r="H69" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>39</v>
+      </c>
+      <c r="B70" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D70" s="47">
+        <v>43397</v>
+      </c>
+      <c r="E70" t="s">
+        <v>57</v>
+      </c>
+      <c r="F70" t="s">
+        <v>1110</v>
+      </c>
+      <c r="G70" s="47">
+        <v>43397</v>
+      </c>
+      <c r="H70" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>39</v>
+      </c>
+      <c r="B71" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D71" s="47">
+        <v>43398</v>
+      </c>
+      <c r="E71" t="s">
+        <v>57</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1093</v>
+      </c>
+      <c r="G71" s="47">
+        <v>43418</v>
+      </c>
+      <c r="H71" t="s">
+        <v>58</v>
+      </c>
+      <c r="J71" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>39</v>
+      </c>
+      <c r="B72" t="s">
+        <v>45</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D72" s="47">
+        <v>43403</v>
+      </c>
+      <c r="E72" t="s">
+        <v>57</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G72" s="47">
+        <v>43418</v>
+      </c>
+      <c r="H72" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73" t="s">
+        <v>78</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D73" s="47">
+        <v>43403</v>
+      </c>
+      <c r="E73" t="s">
+        <v>58</v>
+      </c>
+      <c r="I73" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74" t="s">
+        <v>64</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D74" s="47">
+        <v>43398</v>
+      </c>
+      <c r="E74" t="s">
+        <v>57</v>
+      </c>
+      <c r="F74" t="s">
+        <v>1111</v>
+      </c>
+      <c r="G74" s="47">
+        <v>43404</v>
+      </c>
+      <c r="H74" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>39</v>
+      </c>
+      <c r="B75" t="s">
+        <v>316</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D75" s="47">
+        <v>43412</v>
+      </c>
+      <c r="E75" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>39</v>
+      </c>
+      <c r="B76" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D76" s="47">
+        <v>43412</v>
+      </c>
+      <c r="E76" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>39</v>
+      </c>
+      <c r="B77" t="s">
+        <v>45</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1179</v>
+      </c>
+      <c r="D77" s="47">
+        <v>43409</v>
+      </c>
+      <c r="E77" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>39</v>
+      </c>
+      <c r="B78" t="s">
+        <v>316</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D78" s="47">
+        <v>43412</v>
+      </c>
+      <c r="E78" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>39</v>
+      </c>
+      <c r="B79" t="s">
+        <v>45</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1180</v>
+      </c>
+      <c r="D79" s="47">
+        <v>43413</v>
+      </c>
+      <c r="E79" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>39</v>
+      </c>
+      <c r="B80" t="s">
+        <v>45</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D80" s="47">
+        <v>43413</v>
+      </c>
+      <c r="E80" t="s">
+        <v>57</v>
+      </c>
+      <c r="F80" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>39</v>
+      </c>
+      <c r="B81" t="s">
+        <v>45</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1182</v>
+      </c>
+      <c r="D81" s="47">
+        <v>43413</v>
+      </c>
+      <c r="E81" t="s">
+        <v>57</v>
+      </c>
+      <c r="F81" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G81" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H81" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>39</v>
+      </c>
+      <c r="B82" t="s">
+        <v>45</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D82" s="47">
+        <v>43413</v>
+      </c>
+      <c r="E82" t="s">
+        <v>74</v>
+      </c>
+      <c r="F82" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G82" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H82" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>39</v>
+      </c>
+      <c r="B83" t="s">
+        <v>45</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D83" s="47">
+        <v>43413</v>
+      </c>
+      <c r="E83" t="s">
+        <v>58</v>
+      </c>
+      <c r="I83" t="s">
+        <v>36</v>
+      </c>
+      <c r="J83" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>39</v>
+      </c>
+      <c r="B84" t="s">
+        <v>316</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D84" s="47">
+        <v>43415</v>
+      </c>
+      <c r="E84" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>39</v>
+      </c>
+      <c r="B85" t="s">
+        <v>45</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1184</v>
+      </c>
+      <c r="D85" s="47">
+        <v>43415</v>
+      </c>
+      <c r="E85" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" t="s">
+        <v>65</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D86" s="47">
+        <v>43416</v>
+      </c>
+      <c r="E86" t="s">
+        <v>74</v>
+      </c>
+      <c r="F86" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G86" s="47">
+        <v>43417</v>
+      </c>
+      <c r="H86" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>39</v>
+      </c>
+      <c r="B87" t="s">
+        <v>65</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D87" s="47">
+        <v>43418</v>
+      </c>
+      <c r="E87" t="s">
+        <v>74</v>
+      </c>
+      <c r="F87" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G87" s="47">
         <v>43419</v>
       </c>
-      <c r="E64" t="s">
-        <v>74</v>
-      </c>
-      <c r="F64" t="s">
-        <v>1134</v>
-      </c>
-      <c r="G64" s="47">
-        <v>43430</v>
-      </c>
-      <c r="H64" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>779</v>
-      </c>
-      <c r="B65" t="s">
-        <v>69</v>
-      </c>
-      <c r="C65" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D65" s="47">
+      <c r="H87" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>39</v>
+      </c>
+      <c r="B88" t="s">
+        <v>45</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D88" s="47">
+        <v>43418</v>
+      </c>
+      <c r="E88" t="s">
+        <v>74</v>
+      </c>
+      <c r="F88" t="s">
+        <v>1191</v>
+      </c>
+      <c r="G88" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H88" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" t="s">
+        <v>45</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D89" s="47">
+        <v>43340</v>
+      </c>
+      <c r="E89" t="s">
+        <v>57</v>
+      </c>
+      <c r="F89" t="s">
+        <v>1192</v>
+      </c>
+      <c r="G89" s="47">
+        <v>43418</v>
+      </c>
+      <c r="H89" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>39</v>
+      </c>
+      <c r="B90" t="s">
+        <v>45</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D90" s="47">
+        <v>43398</v>
+      </c>
+      <c r="E90" t="s">
+        <v>74</v>
+      </c>
+      <c r="F90" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G90" s="47">
         <v>43419</v>
       </c>
-      <c r="E65" t="s">
-        <v>74</v>
-      </c>
-      <c r="F65" t="s">
-        <v>1136</v>
-      </c>
-      <c r="G65" s="47">
-        <v>43430</v>
-      </c>
-      <c r="H65" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>779</v>
-      </c>
-      <c r="B66" t="s">
-        <v>69</v>
-      </c>
-      <c r="C66" t="s">
-        <v>1137</v>
-      </c>
-      <c r="D66" s="47">
-        <v>43430</v>
-      </c>
-      <c r="E66" t="s">
-        <v>74</v>
-      </c>
-      <c r="F66" t="s">
-        <v>1138</v>
-      </c>
-      <c r="G66" s="47">
+      <c r="H90" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>39</v>
+      </c>
+      <c r="B91" t="s">
+        <v>45</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D91" s="47">
+        <v>43402</v>
+      </c>
+      <c r="E91" t="s">
+        <v>74</v>
+      </c>
+      <c r="F91" t="s">
+        <v>1194</v>
+      </c>
+      <c r="G91" s="47">
+        <v>43418</v>
+      </c>
+      <c r="H91" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>39</v>
+      </c>
+      <c r="B92" t="s">
+        <v>45</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D92" s="47">
+        <v>43419</v>
+      </c>
+      <c r="E92" t="s">
+        <v>74</v>
+      </c>
+      <c r="F92" t="s">
+        <v>1195</v>
+      </c>
+      <c r="G92" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H92" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>39</v>
+      </c>
+      <c r="B93" t="s">
+        <v>45</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D93" s="47">
+        <v>43419</v>
+      </c>
+      <c r="E93" t="s">
+        <v>74</v>
+      </c>
+      <c r="F93" t="s">
+        <v>1196</v>
+      </c>
+      <c r="G93" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H93" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>39</v>
+      </c>
+      <c r="B94" t="s">
+        <v>45</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D94" s="47">
+        <v>43419</v>
+      </c>
+      <c r="E94" t="s">
+        <v>74</v>
+      </c>
+      <c r="F94" t="s">
+        <v>1197</v>
+      </c>
+      <c r="G94" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H94" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>39</v>
+      </c>
+      <c r="B95" t="s">
+        <v>45</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D95" s="47">
+        <v>43419</v>
+      </c>
+      <c r="E95" t="s">
+        <v>74</v>
+      </c>
+      <c r="F95" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G95" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H95" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>39</v>
+      </c>
+      <c r="B96" t="s">
+        <v>45</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D96" s="47">
+        <v>43419</v>
+      </c>
+      <c r="E96" t="s">
+        <v>74</v>
+      </c>
+      <c r="F96" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G96" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H96" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B97" t="s">
+        <v>45</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D97" s="47">
+        <v>43419</v>
+      </c>
+      <c r="E97" t="s">
+        <v>74</v>
+      </c>
+      <c r="F97" t="s">
+        <v>1200</v>
+      </c>
+      <c r="G97" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H97" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>39</v>
+      </c>
+      <c r="B98" t="s">
+        <v>45</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D98" s="47">
+        <v>43419</v>
+      </c>
+      <c r="E98" t="s">
+        <v>74</v>
+      </c>
+      <c r="F98" t="s">
+        <v>1201</v>
+      </c>
+      <c r="G98" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H98" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>39</v>
+      </c>
+      <c r="B99" t="s">
+        <v>45</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1202</v>
+      </c>
+      <c r="D99" s="47">
+        <v>43419</v>
+      </c>
+      <c r="E99" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>39</v>
+      </c>
+      <c r="B100" t="s">
+        <v>65</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D100" s="47">
+        <v>43418</v>
+      </c>
+      <c r="E100" t="s">
+        <v>74</v>
+      </c>
+      <c r="F100" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G100" s="47">
+        <v>43431</v>
+      </c>
+      <c r="H100" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>39</v>
+      </c>
+      <c r="B101" t="s">
+        <v>45</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1203</v>
+      </c>
+      <c r="D101" s="47">
+        <v>43431</v>
+      </c>
+      <c r="E101" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>39</v>
+      </c>
+      <c r="B102" t="s">
+        <v>45</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D102" s="47">
+        <v>43431</v>
+      </c>
+      <c r="E102" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>39</v>
+      </c>
+      <c r="B103" t="s">
+        <v>45</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1205</v>
+      </c>
+      <c r="D103" s="47">
+        <v>43431</v>
+      </c>
+      <c r="E103" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>39</v>
+      </c>
+      <c r="B104" t="s">
+        <v>45</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D104" s="47">
+        <v>43431</v>
+      </c>
+      <c r="E104" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>39</v>
+      </c>
+      <c r="B105" t="s">
+        <v>45</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1207</v>
+      </c>
+      <c r="D105" s="47">
+        <v>43431</v>
+      </c>
+      <c r="E105" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>39</v>
+      </c>
+      <c r="B106" t="s">
+        <v>45</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1208</v>
+      </c>
+      <c r="D106" s="47">
+        <v>43431</v>
+      </c>
+      <c r="E106" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>39</v>
+      </c>
+      <c r="B107" t="s">
+        <v>45</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D107" s="47">
+        <v>43431</v>
+      </c>
+      <c r="E107" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>39</v>
+      </c>
+      <c r="B108" t="s">
+        <v>45</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D108" s="47">
+        <v>43431</v>
+      </c>
+      <c r="E108" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>39</v>
+      </c>
+      <c r="B109" t="s">
+        <v>45</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1211</v>
+      </c>
+      <c r="D109" s="47">
+        <v>43431</v>
+      </c>
+      <c r="E109" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>39</v>
+      </c>
+      <c r="B110" t="s">
+        <v>45</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D110" s="47">
+        <v>43431</v>
+      </c>
+      <c r="E110" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>39</v>
+      </c>
+      <c r="B111" t="s">
+        <v>45</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1213</v>
+      </c>
+      <c r="D111" s="47">
+        <v>43432</v>
+      </c>
+      <c r="E111" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>39</v>
+      </c>
+      <c r="B112" t="s">
+        <v>45</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1214</v>
+      </c>
+      <c r="D112" s="47">
         <v>43433</v>
       </c>
-      <c r="H66" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>779</v>
-      </c>
-      <c r="B67" t="s">
-        <v>69</v>
-      </c>
-      <c r="C67" t="s">
-        <v>1139</v>
-      </c>
-      <c r="D67" s="47">
-        <v>43418</v>
-      </c>
-      <c r="E67" t="s">
-        <v>74</v>
-      </c>
-      <c r="F67" t="s">
-        <v>1140</v>
-      </c>
-      <c r="G67" s="47">
-        <v>43430</v>
-      </c>
-      <c r="H67" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>779</v>
-      </c>
-      <c r="B68" t="s">
-        <v>69</v>
-      </c>
-      <c r="C68" t="s">
-        <v>1141</v>
-      </c>
-      <c r="D68" s="47">
-        <v>43417</v>
-      </c>
-      <c r="E68" t="s">
-        <v>74</v>
-      </c>
-      <c r="F68" t="s">
-        <v>1142</v>
-      </c>
-      <c r="G68" s="47">
-        <v>43430</v>
-      </c>
-      <c r="H68" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>779</v>
-      </c>
-      <c r="B69" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" t="s">
-        <v>1143</v>
-      </c>
-      <c r="D69" s="47">
-        <v>43419</v>
-      </c>
-      <c r="E69" t="s">
-        <v>74</v>
-      </c>
-      <c r="F69" t="s">
-        <v>1144</v>
-      </c>
-      <c r="G69" s="47">
-        <v>43430</v>
-      </c>
-      <c r="H69" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>779</v>
-      </c>
-      <c r="B70" t="s">
-        <v>69</v>
-      </c>
-      <c r="C70" t="s">
-        <v>1145</v>
-      </c>
-      <c r="D70" s="47">
-        <v>43419</v>
-      </c>
-      <c r="E70" t="s">
-        <v>74</v>
-      </c>
-      <c r="F70" t="s">
-        <v>1146</v>
-      </c>
-      <c r="G70" s="47">
-        <v>43430</v>
-      </c>
-      <c r="H70" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>779</v>
-      </c>
-      <c r="B71" t="s">
-        <v>69</v>
-      </c>
-      <c r="C71" t="s">
-        <v>1147</v>
-      </c>
-      <c r="D71" s="47">
-        <v>43430</v>
-      </c>
-      <c r="E71" t="s">
-        <v>74</v>
-      </c>
-      <c r="F71" t="s">
-        <v>1148</v>
-      </c>
-      <c r="G71" s="47">
-        <v>43434</v>
-      </c>
-      <c r="H71" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>779</v>
-      </c>
-      <c r="B72" t="s">
-        <v>69</v>
-      </c>
-      <c r="C72" t="s">
-        <v>1149</v>
-      </c>
-      <c r="D72" s="47">
-        <v>43430</v>
-      </c>
-      <c r="E72" t="s">
-        <v>74</v>
-      </c>
-      <c r="F72" t="s">
-        <v>1149</v>
-      </c>
-      <c r="G72" s="47">
-        <v>43434</v>
-      </c>
-      <c r="H72" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>779</v>
-      </c>
-      <c r="B73" t="s">
-        <v>69</v>
-      </c>
-      <c r="C73" t="s">
-        <v>1150</v>
-      </c>
-      <c r="D73" s="47">
-        <v>43430</v>
-      </c>
-      <c r="E73" t="s">
-        <v>74</v>
-      </c>
-      <c r="F73" t="s">
-        <v>1138</v>
-      </c>
-      <c r="G73" s="47">
+      <c r="E112" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>39</v>
+      </c>
+      <c r="B113" t="s">
+        <v>45</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1215</v>
+      </c>
+      <c r="D113" s="47">
         <v>43433</v>
       </c>
-      <c r="H73" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>779</v>
-      </c>
-      <c r="B74" t="s">
-        <v>69</v>
-      </c>
-      <c r="C74" t="s">
-        <v>1151</v>
-      </c>
-      <c r="D74" s="47">
-        <v>43433</v>
-      </c>
-      <c r="E74" t="s">
-        <v>74</v>
-      </c>
-      <c r="F74" t="s">
-        <v>1152</v>
-      </c>
-      <c r="G74" s="47">
-        <v>43434</v>
-      </c>
-      <c r="H74" t="s">
+      <c r="E113" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>39</v>
+      </c>
+      <c r="B114" t="s">
+        <v>45</v>
+      </c>
+      <c r="C114" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D114" s="47">
+        <v>43340</v>
+      </c>
+      <c r="E114" t="s">
+        <v>74</v>
+      </c>
+      <c r="F114" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G114" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H114" t="s">
+        <v>58</v>
+      </c>
+      <c r="I114" t="s">
+        <v>36</v>
+      </c>
+      <c r="J114" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>39</v>
+      </c>
+      <c r="B115" t="s">
+        <v>45</v>
+      </c>
+      <c r="C115" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D115" s="47">
+        <v>43340</v>
+      </c>
+      <c r="E115" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>39</v>
+      </c>
+      <c r="B116" t="s">
+        <v>45</v>
+      </c>
+      <c r="C116" t="s">
+        <v>1218</v>
+      </c>
+      <c r="D116" s="47">
+        <v>43308</v>
+      </c>
+      <c r="E116" t="s">
+        <v>74</v>
+      </c>
+      <c r="F116" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G116" s="47">
+        <v>43437</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>39</v>
+      </c>
+      <c r="B117" t="s">
+        <v>45</v>
+      </c>
+      <c r="C117" t="s">
+        <v>1219</v>
+      </c>
+      <c r="D117" s="47">
+        <v>43339</v>
+      </c>
+      <c r="E117" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>39</v>
+      </c>
+      <c r="B118" t="s">
+        <v>45</v>
+      </c>
+      <c r="C118" t="s">
+        <v>1220</v>
+      </c>
+      <c r="D118" s="47">
+        <v>43334</v>
+      </c>
+      <c r="E118" t="s">
+        <v>74</v>
+      </c>
+      <c r="F118" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G118" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H118" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>39</v>
+      </c>
+      <c r="B119" t="s">
+        <v>45</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D119" s="47">
+        <v>43384</v>
+      </c>
+      <c r="E119" t="s">
+        <v>74</v>
+      </c>
+      <c r="F119" t="s">
+        <v>1221</v>
+      </c>
+      <c r="G119" s="47">
+        <v>43437</v>
+      </c>
+      <c r="H119" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:J74">
+    <sortCondition ref="A2:A74"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>SQA!$A$1:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Application!$A$2:$A$62</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>'A or D'!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1048576 H2:H1048576</xm:sqref>
+          <xm:sqref>H2:H1048576 E1:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>'Reasons for Disapproval'!$A$1:$A$14</xm:f>
           </x14:formula1>
@@ -6022,11 +7275,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2157" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2178" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2187" sqref="A2187"/>
     </sheetView>
   </sheetViews>
@@ -67382,7 +68635,7 @@
     <sortCondition ref="H793:H798"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1347">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1347" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$A$2:$A$54</formula1>
     </dataValidation>
   </dataValidations>
@@ -67394,109 +68647,109 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="18">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'A or D'!$A$1:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G315 G317:G661 G671:G924 G926:G1197 G1208:G1579 G1589:G1765 G1801:G2066 G2079:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 282018.xlsx]A or D'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G316</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>SQA!$A$1:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A661 A671:A924 A926:A1197 A1208:A1579 A1589:A1765 A1801:A2066 A2079:A1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>'Deliverable Types'!$A$1:$A$31</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D661 D671:D924 D926:D1197 D1208:D1579 D1589:D1765 D1801:D2066 D2079:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>'C:\Users\lauernd\Desktop\[Nick First Pass Acceptance.xlsx]Deliverable Types'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D662:D670 D1198:D1207 D925</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>'C:\Users\lauernd\Desktop\[Nick First Pass Acceptance.xlsx]A or D'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G662:G670 G1198:G1207 G925</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>'C:\Users\lauernd\Desktop\[Nick First Pass Acceptance.xlsx]SQA'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>A662:A670 A1198:A1207 A925</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 9142018.xlsx]Deliverable Types'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D1580:D1588</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 9142018.xlsx]A or D'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G1580:G1588</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 9142018.xlsx]SQA'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>A1580:A1588</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
           <x14:formula1>
             <xm:f>Application!$A$2:$A$62</xm:f>
           </x14:formula1>
           <xm:sqref>C1:C1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 10052018.xlsx]Deliverable Types'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D1766:D1800</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 10052018.xlsx]SQA'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>A1766:A1800</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000E000000}">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 10052018.xlsx]A or D'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G1766:G1800</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000F000000}">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 11092018.xlsx]Deliverable Types'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D2067:D2078</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000010000000}">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 11092018.xlsx]SQA'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>A2067:A2078</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000011000000}">
           <x14:formula1>
             <xm:f>'[First Pass Acceptance_Beilah 11092018.xlsx]A or D'!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>G2067:G2078</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000012000000}">
           <x14:formula1>
             <xm:f>'Reasons for Disapproval'!$A$1:$A$14</xm:f>
           </x14:formula1>
@@ -67509,7 +68762,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -67544,7 +68797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A62"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
@@ -67867,7 +69120,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A61"/>
+  <autoFilter ref="A1:A61" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <sortState ref="A2:A62">
     <sortCondition ref="A2:A62"/>
   </sortState>
@@ -67877,7 +69130,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -68054,7 +69307,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -68145,7 +69398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>